<commit_message>
Update test sets for initial run
</commit_message>
<xml_diff>
--- a/attendance/src/main/resources/LeaveDeductions.xlsx
+++ b/attendance/src/main/resources/LeaveDeductions.xlsx
@@ -1271,12 +1271,12 @@
     </xf>
   </cellXfs>
   <cellStyles count="6">
-    <cellStyle name="Normal" xfId="0" builtinId="0"/>
-    <cellStyle name="Comma" xfId="15" builtinId="3"/>
-    <cellStyle name="Comma [0]" xfId="16" builtinId="6"/>
-    <cellStyle name="Currency" xfId="17" builtinId="4"/>
-    <cellStyle name="Currency [0]" xfId="18" builtinId="7"/>
-    <cellStyle name="Percent" xfId="19" builtinId="5"/>
+    <cellStyle name="Normal" xfId="0" builtinId="0" customBuiltin="false"/>
+    <cellStyle name="Comma" xfId="15" builtinId="3" customBuiltin="false"/>
+    <cellStyle name="Comma [0]" xfId="16" builtinId="6" customBuiltin="false"/>
+    <cellStyle name="Currency" xfId="17" builtinId="4" customBuiltin="false"/>
+    <cellStyle name="Currency [0]" xfId="18" builtinId="7" customBuiltin="false"/>
+    <cellStyle name="Percent" xfId="19" builtinId="5" customBuiltin="false"/>
   </cellStyles>
 </styleSheet>
 </file>
@@ -1286,10 +1286,10 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:H268"/>
+  <dimension ref="A1:H1048576"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="D103" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="E112" activeCellId="0" sqref="E112:E118"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A8" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="C29" activeCellId="0" sqref="C29"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -4372,756 +4372,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="119" customFormat="false" ht="12.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A119" s="2"/>
-      <c r="B119" s="2"/>
-      <c r="C119" s="2"/>
-    </row>
-    <row r="120" customFormat="false" ht="12.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A120" s="2"/>
-      <c r="B120" s="2"/>
-      <c r="C120" s="2"/>
-    </row>
-    <row r="121" customFormat="false" ht="12.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A121" s="2"/>
-      <c r="B121" s="2"/>
-      <c r="C121" s="2"/>
-    </row>
-    <row r="122" customFormat="false" ht="12.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A122" s="2"/>
-      <c r="B122" s="2"/>
-      <c r="C122" s="2"/>
-    </row>
-    <row r="123" customFormat="false" ht="12.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A123" s="2"/>
-      <c r="B123" s="2"/>
-      <c r="C123" s="2"/>
-    </row>
-    <row r="124" customFormat="false" ht="12.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A124" s="2"/>
-      <c r="B124" s="2"/>
-      <c r="C124" s="2"/>
-    </row>
-    <row r="125" customFormat="false" ht="12.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A125" s="2"/>
-      <c r="B125" s="2"/>
-      <c r="C125" s="2"/>
-    </row>
-    <row r="126" customFormat="false" ht="12.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A126" s="2"/>
-      <c r="B126" s="2"/>
-      <c r="C126" s="2"/>
-    </row>
-    <row r="127" customFormat="false" ht="12.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A127" s="2"/>
-      <c r="B127" s="2"/>
-      <c r="C127" s="2"/>
-    </row>
-    <row r="128" customFormat="false" ht="12.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A128" s="2"/>
-      <c r="B128" s="2"/>
-      <c r="C128" s="2"/>
-    </row>
-    <row r="129" customFormat="false" ht="12.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A129" s="2"/>
-      <c r="B129" s="2"/>
-      <c r="C129" s="2"/>
-    </row>
-    <row r="130" customFormat="false" ht="12.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A130" s="2"/>
-      <c r="B130" s="2"/>
-      <c r="C130" s="2"/>
-    </row>
-    <row r="131" customFormat="false" ht="12.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A131" s="2"/>
-      <c r="B131" s="2"/>
-      <c r="C131" s="2"/>
-    </row>
-    <row r="132" customFormat="false" ht="12.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A132" s="2"/>
-      <c r="B132" s="2"/>
-      <c r="C132" s="2"/>
-    </row>
-    <row r="133" customFormat="false" ht="12.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A133" s="2"/>
-      <c r="B133" s="2"/>
-      <c r="C133" s="2"/>
-    </row>
-    <row r="134" customFormat="false" ht="12.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A134" s="2"/>
-      <c r="B134" s="2"/>
-      <c r="C134" s="2"/>
-    </row>
-    <row r="135" customFormat="false" ht="12.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A135" s="2"/>
-      <c r="B135" s="2"/>
-      <c r="C135" s="2"/>
-    </row>
-    <row r="136" customFormat="false" ht="12.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A136" s="2"/>
-      <c r="B136" s="2"/>
-      <c r="C136" s="2"/>
-    </row>
-    <row r="137" customFormat="false" ht="12.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A137" s="2"/>
-      <c r="B137" s="2"/>
-      <c r="C137" s="2"/>
-    </row>
-    <row r="138" customFormat="false" ht="12.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A138" s="2"/>
-      <c r="B138" s="2"/>
-      <c r="C138" s="2"/>
-    </row>
-    <row r="139" customFormat="false" ht="12.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A139" s="2"/>
-      <c r="B139" s="2"/>
-      <c r="C139" s="2"/>
-    </row>
-    <row r="140" customFormat="false" ht="12.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A140" s="2"/>
-      <c r="B140" s="2"/>
-      <c r="C140" s="2"/>
-    </row>
-    <row r="141" customFormat="false" ht="12.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A141" s="2"/>
-      <c r="B141" s="2"/>
-      <c r="C141" s="2"/>
-    </row>
-    <row r="142" customFormat="false" ht="12.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A142" s="2"/>
-      <c r="B142" s="2"/>
-      <c r="C142" s="2"/>
-    </row>
-    <row r="143" customFormat="false" ht="12.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A143" s="2"/>
-      <c r="B143" s="2"/>
-      <c r="C143" s="2"/>
-    </row>
-    <row r="144" customFormat="false" ht="12.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A144" s="2"/>
-      <c r="B144" s="2"/>
-      <c r="C144" s="2"/>
-    </row>
-    <row r="145" customFormat="false" ht="12.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A145" s="2"/>
-      <c r="B145" s="2"/>
-      <c r="C145" s="2"/>
-    </row>
-    <row r="146" customFormat="false" ht="12.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A146" s="2"/>
-      <c r="B146" s="2"/>
-      <c r="C146" s="2"/>
-    </row>
-    <row r="147" customFormat="false" ht="12.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A147" s="2"/>
-      <c r="B147" s="2"/>
-      <c r="C147" s="2"/>
-    </row>
-    <row r="148" customFormat="false" ht="12.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A148" s="2"/>
-      <c r="B148" s="2"/>
-      <c r="C148" s="2"/>
-    </row>
-    <row r="149" customFormat="false" ht="12.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A149" s="2"/>
-      <c r="B149" s="2"/>
-      <c r="C149" s="2"/>
-    </row>
-    <row r="150" customFormat="false" ht="12.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A150" s="2"/>
-      <c r="B150" s="2"/>
-      <c r="C150" s="2"/>
-    </row>
-    <row r="151" customFormat="false" ht="12.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A151" s="2"/>
-      <c r="B151" s="2"/>
-      <c r="C151" s="2"/>
-    </row>
-    <row r="152" customFormat="false" ht="12.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A152" s="2"/>
-      <c r="B152" s="2"/>
-      <c r="C152" s="2"/>
-    </row>
-    <row r="153" customFormat="false" ht="12.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A153" s="2"/>
-      <c r="B153" s="2"/>
-      <c r="C153" s="2"/>
-    </row>
-    <row r="154" customFormat="false" ht="12.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A154" s="2"/>
-      <c r="B154" s="2"/>
-      <c r="C154" s="2"/>
-    </row>
-    <row r="155" customFormat="false" ht="12.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A155" s="2"/>
-      <c r="B155" s="2"/>
-      <c r="C155" s="2"/>
-    </row>
-    <row r="156" customFormat="false" ht="12.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A156" s="2"/>
-      <c r="B156" s="2"/>
-      <c r="C156" s="2"/>
-    </row>
-    <row r="157" customFormat="false" ht="12.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A157" s="2"/>
-      <c r="B157" s="2"/>
-      <c r="C157" s="2"/>
-    </row>
-    <row r="158" customFormat="false" ht="12.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A158" s="2"/>
-      <c r="B158" s="2"/>
-      <c r="C158" s="2"/>
-    </row>
-    <row r="159" customFormat="false" ht="12.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A159" s="2"/>
-      <c r="B159" s="2"/>
-      <c r="C159" s="2"/>
-    </row>
-    <row r="160" customFormat="false" ht="12.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A160" s="2"/>
-      <c r="B160" s="2"/>
-      <c r="C160" s="2"/>
-    </row>
-    <row r="161" customFormat="false" ht="12.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A161" s="2"/>
-      <c r="B161" s="2"/>
-      <c r="C161" s="2"/>
-    </row>
-    <row r="162" customFormat="false" ht="12.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A162" s="2"/>
-      <c r="B162" s="2"/>
-      <c r="C162" s="2"/>
-    </row>
-    <row r="163" customFormat="false" ht="12.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A163" s="2"/>
-      <c r="B163" s="2"/>
-      <c r="C163" s="2"/>
-    </row>
-    <row r="164" customFormat="false" ht="12.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A164" s="2"/>
-      <c r="B164" s="2"/>
-      <c r="C164" s="2"/>
-    </row>
-    <row r="165" customFormat="false" ht="12.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A165" s="2"/>
-      <c r="B165" s="2"/>
-      <c r="C165" s="2"/>
-    </row>
-    <row r="166" customFormat="false" ht="12.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A166" s="2"/>
-      <c r="B166" s="2"/>
-      <c r="C166" s="2"/>
-    </row>
-    <row r="167" customFormat="false" ht="12.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A167" s="2"/>
-      <c r="B167" s="2"/>
-      <c r="C167" s="2"/>
-    </row>
-    <row r="168" customFormat="false" ht="12.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A168" s="2"/>
-      <c r="B168" s="2"/>
-      <c r="C168" s="2"/>
-    </row>
-    <row r="169" customFormat="false" ht="12.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A169" s="2"/>
-      <c r="B169" s="2"/>
-      <c r="C169" s="2"/>
-    </row>
-    <row r="170" customFormat="false" ht="12.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A170" s="2"/>
-      <c r="B170" s="2"/>
-      <c r="C170" s="2"/>
-    </row>
-    <row r="171" customFormat="false" ht="12.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A171" s="2"/>
-      <c r="B171" s="2"/>
-      <c r="C171" s="2"/>
-    </row>
-    <row r="172" customFormat="false" ht="12.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A172" s="2"/>
-      <c r="B172" s="2"/>
-      <c r="C172" s="2"/>
-    </row>
-    <row r="173" customFormat="false" ht="12.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A173" s="2"/>
-      <c r="B173" s="2"/>
-      <c r="C173" s="2"/>
-    </row>
-    <row r="174" customFormat="false" ht="12.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A174" s="2"/>
-      <c r="B174" s="2"/>
-      <c r="C174" s="2"/>
-    </row>
-    <row r="175" customFormat="false" ht="12.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A175" s="2"/>
-      <c r="B175" s="2"/>
-      <c r="C175" s="2"/>
-    </row>
-    <row r="176" customFormat="false" ht="12.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A176" s="2"/>
-      <c r="B176" s="2"/>
-      <c r="C176" s="2"/>
-    </row>
-    <row r="177" customFormat="false" ht="12.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A177" s="2"/>
-      <c r="B177" s="2"/>
-      <c r="C177" s="2"/>
-    </row>
-    <row r="178" customFormat="false" ht="12.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A178" s="2"/>
-      <c r="B178" s="2"/>
-      <c r="C178" s="2"/>
-    </row>
-    <row r="179" customFormat="false" ht="12.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A179" s="2"/>
-      <c r="B179" s="2"/>
-      <c r="C179" s="2"/>
-    </row>
-    <row r="180" customFormat="false" ht="12.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A180" s="2"/>
-      <c r="B180" s="2"/>
-      <c r="C180" s="2"/>
-    </row>
-    <row r="181" customFormat="false" ht="12.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A181" s="2"/>
-      <c r="B181" s="2"/>
-      <c r="C181" s="2"/>
-    </row>
-    <row r="182" customFormat="false" ht="12.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A182" s="2"/>
-      <c r="B182" s="2"/>
-      <c r="C182" s="2"/>
-    </row>
-    <row r="183" customFormat="false" ht="12.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A183" s="2"/>
-      <c r="B183" s="2"/>
-      <c r="C183" s="2"/>
-    </row>
-    <row r="184" customFormat="false" ht="12.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A184" s="2"/>
-      <c r="B184" s="2"/>
-      <c r="C184" s="2"/>
-    </row>
-    <row r="185" customFormat="false" ht="12.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A185" s="2"/>
-      <c r="B185" s="2"/>
-      <c r="C185" s="2"/>
-    </row>
-    <row r="186" customFormat="false" ht="12.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A186" s="2"/>
-      <c r="B186" s="2"/>
-      <c r="C186" s="2"/>
-    </row>
-    <row r="187" customFormat="false" ht="12.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A187" s="2"/>
-      <c r="B187" s="2"/>
-      <c r="C187" s="2"/>
-    </row>
-    <row r="188" customFormat="false" ht="12.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A188" s="2"/>
-      <c r="B188" s="2"/>
-      <c r="C188" s="2"/>
-    </row>
-    <row r="189" customFormat="false" ht="12.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A189" s="2"/>
-      <c r="B189" s="2"/>
-      <c r="C189" s="2"/>
-    </row>
-    <row r="190" customFormat="false" ht="12.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A190" s="2"/>
-      <c r="B190" s="2"/>
-      <c r="C190" s="2"/>
-    </row>
-    <row r="191" customFormat="false" ht="12.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A191" s="2"/>
-      <c r="B191" s="2"/>
-      <c r="C191" s="2"/>
-    </row>
-    <row r="192" customFormat="false" ht="12.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A192" s="2"/>
-      <c r="B192" s="2"/>
-      <c r="C192" s="2"/>
-    </row>
-    <row r="193" customFormat="false" ht="12.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A193" s="2"/>
-      <c r="B193" s="2"/>
-      <c r="C193" s="2"/>
-    </row>
-    <row r="194" customFormat="false" ht="12.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A194" s="2"/>
-      <c r="B194" s="2"/>
-      <c r="C194" s="2"/>
-    </row>
-    <row r="195" customFormat="false" ht="12.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A195" s="2"/>
-      <c r="B195" s="2"/>
-      <c r="C195" s="2"/>
-    </row>
-    <row r="196" customFormat="false" ht="12.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A196" s="2"/>
-      <c r="B196" s="2"/>
-      <c r="C196" s="2"/>
-    </row>
-    <row r="197" customFormat="false" ht="12.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A197" s="2"/>
-      <c r="B197" s="2"/>
-      <c r="C197" s="2"/>
-    </row>
-    <row r="198" customFormat="false" ht="12.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A198" s="2"/>
-      <c r="B198" s="2"/>
-      <c r="C198" s="2"/>
-    </row>
-    <row r="199" customFormat="false" ht="12.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A199" s="2"/>
-      <c r="B199" s="2"/>
-      <c r="C199" s="2"/>
-    </row>
-    <row r="200" customFormat="false" ht="12.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A200" s="2"/>
-      <c r="B200" s="2"/>
-      <c r="C200" s="2"/>
-    </row>
-    <row r="201" customFormat="false" ht="12.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A201" s="2"/>
-      <c r="B201" s="2"/>
-      <c r="C201" s="2"/>
-    </row>
-    <row r="202" customFormat="false" ht="12.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A202" s="2"/>
-      <c r="B202" s="2"/>
-      <c r="C202" s="2"/>
-    </row>
-    <row r="203" customFormat="false" ht="12.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A203" s="2"/>
-      <c r="B203" s="2"/>
-      <c r="C203" s="2"/>
-    </row>
-    <row r="204" customFormat="false" ht="12.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A204" s="2"/>
-      <c r="B204" s="2"/>
-      <c r="C204" s="2"/>
-    </row>
-    <row r="205" customFormat="false" ht="12.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A205" s="2"/>
-      <c r="B205" s="2"/>
-      <c r="C205" s="2"/>
-    </row>
-    <row r="206" customFormat="false" ht="12.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A206" s="2"/>
-      <c r="B206" s="2"/>
-      <c r="C206" s="2"/>
-    </row>
-    <row r="207" customFormat="false" ht="12.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A207" s="2"/>
-      <c r="B207" s="2"/>
-      <c r="C207" s="2"/>
-    </row>
-    <row r="208" customFormat="false" ht="12.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A208" s="2"/>
-      <c r="B208" s="2"/>
-      <c r="C208" s="2"/>
-    </row>
-    <row r="209" customFormat="false" ht="12.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A209" s="2"/>
-      <c r="B209" s="2"/>
-      <c r="C209" s="2"/>
-    </row>
-    <row r="210" customFormat="false" ht="12.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A210" s="2"/>
-      <c r="B210" s="2"/>
-      <c r="C210" s="2"/>
-    </row>
-    <row r="211" customFormat="false" ht="12.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A211" s="2"/>
-      <c r="B211" s="2"/>
-      <c r="C211" s="2"/>
-    </row>
-    <row r="212" customFormat="false" ht="12.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A212" s="2"/>
-      <c r="B212" s="2"/>
-      <c r="C212" s="2"/>
-    </row>
-    <row r="213" customFormat="false" ht="12.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A213" s="2"/>
-      <c r="B213" s="2"/>
-      <c r="C213" s="2"/>
-    </row>
-    <row r="214" customFormat="false" ht="12.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A214" s="2"/>
-      <c r="B214" s="2"/>
-      <c r="C214" s="2"/>
-    </row>
-    <row r="215" customFormat="false" ht="12.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A215" s="2"/>
-      <c r="B215" s="2"/>
-      <c r="C215" s="2"/>
-    </row>
-    <row r="216" customFormat="false" ht="12.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A216" s="2"/>
-      <c r="B216" s="2"/>
-      <c r="C216" s="2"/>
-    </row>
-    <row r="217" customFormat="false" ht="12.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A217" s="2"/>
-      <c r="B217" s="2"/>
-      <c r="C217" s="2"/>
-    </row>
-    <row r="218" customFormat="false" ht="12.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A218" s="2"/>
-      <c r="B218" s="2"/>
-      <c r="C218" s="2"/>
-    </row>
-    <row r="219" customFormat="false" ht="12.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A219" s="2"/>
-      <c r="B219" s="2"/>
-      <c r="C219" s="2"/>
-    </row>
-    <row r="220" customFormat="false" ht="12.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A220" s="2"/>
-      <c r="B220" s="2"/>
-      <c r="C220" s="2"/>
-    </row>
-    <row r="221" customFormat="false" ht="12.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A221" s="2"/>
-      <c r="B221" s="2"/>
-      <c r="C221" s="2"/>
-    </row>
-    <row r="222" customFormat="false" ht="12.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A222" s="2"/>
-      <c r="B222" s="2"/>
-      <c r="C222" s="2"/>
-    </row>
-    <row r="223" customFormat="false" ht="12.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A223" s="2"/>
-      <c r="B223" s="2"/>
-      <c r="C223" s="2"/>
-    </row>
-    <row r="224" customFormat="false" ht="12.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A224" s="2"/>
-      <c r="B224" s="2"/>
-      <c r="C224" s="2"/>
-    </row>
-    <row r="225" customFormat="false" ht="12.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A225" s="2"/>
-      <c r="B225" s="2"/>
-      <c r="C225" s="2"/>
-    </row>
-    <row r="226" customFormat="false" ht="12.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A226" s="2"/>
-      <c r="B226" s="2"/>
-      <c r="C226" s="2"/>
-    </row>
-    <row r="227" customFormat="false" ht="12.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A227" s="2"/>
-      <c r="B227" s="2"/>
-      <c r="C227" s="2"/>
-    </row>
-    <row r="228" customFormat="false" ht="12.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A228" s="2"/>
-      <c r="B228" s="2"/>
-      <c r="C228" s="2"/>
-    </row>
-    <row r="229" customFormat="false" ht="12.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A229" s="2"/>
-      <c r="B229" s="2"/>
-      <c r="C229" s="2"/>
-    </row>
-    <row r="230" customFormat="false" ht="12.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A230" s="2"/>
-      <c r="B230" s="2"/>
-      <c r="C230" s="2"/>
-    </row>
-    <row r="231" customFormat="false" ht="12.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A231" s="2"/>
-      <c r="B231" s="2"/>
-      <c r="C231" s="2"/>
-    </row>
-    <row r="232" customFormat="false" ht="12.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A232" s="2"/>
-      <c r="B232" s="2"/>
-      <c r="C232" s="2"/>
-    </row>
-    <row r="233" customFormat="false" ht="12.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A233" s="2"/>
-      <c r="B233" s="2"/>
-      <c r="C233" s="2"/>
-    </row>
-    <row r="234" customFormat="false" ht="12.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A234" s="2"/>
-      <c r="B234" s="2"/>
-      <c r="C234" s="2"/>
-    </row>
-    <row r="235" customFormat="false" ht="12.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A235" s="2"/>
-      <c r="B235" s="2"/>
-      <c r="C235" s="2"/>
-    </row>
-    <row r="236" customFormat="false" ht="12.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A236" s="2"/>
-      <c r="B236" s="2"/>
-      <c r="C236" s="2"/>
-    </row>
-    <row r="237" customFormat="false" ht="12.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A237" s="2"/>
-      <c r="B237" s="2"/>
-      <c r="C237" s="2"/>
-    </row>
-    <row r="238" customFormat="false" ht="12.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A238" s="2"/>
-      <c r="B238" s="2"/>
-      <c r="C238" s="2"/>
-    </row>
-    <row r="239" customFormat="false" ht="12.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A239" s="2"/>
-      <c r="B239" s="2"/>
-      <c r="C239" s="2"/>
-    </row>
-    <row r="240" customFormat="false" ht="12.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A240" s="2"/>
-      <c r="B240" s="2"/>
-      <c r="C240" s="2"/>
-    </row>
-    <row r="241" customFormat="false" ht="12.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A241" s="2"/>
-      <c r="B241" s="2"/>
-      <c r="C241" s="2"/>
-    </row>
-    <row r="242" customFormat="false" ht="12.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A242" s="2"/>
-      <c r="B242" s="2"/>
-      <c r="C242" s="2"/>
-    </row>
-    <row r="243" customFormat="false" ht="12.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A243" s="2"/>
-      <c r="B243" s="2"/>
-      <c r="C243" s="2"/>
-    </row>
-    <row r="244" customFormat="false" ht="12.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A244" s="2"/>
-      <c r="B244" s="2"/>
-      <c r="C244" s="2"/>
-    </row>
-    <row r="245" customFormat="false" ht="12.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A245" s="2"/>
-      <c r="B245" s="2"/>
-      <c r="C245" s="2"/>
-    </row>
-    <row r="246" customFormat="false" ht="12.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A246" s="2"/>
-      <c r="B246" s="2"/>
-      <c r="C246" s="2"/>
-    </row>
-    <row r="247" customFormat="false" ht="12.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A247" s="2"/>
-      <c r="B247" s="2"/>
-      <c r="C247" s="2"/>
-    </row>
-    <row r="248" customFormat="false" ht="12.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A248" s="2"/>
-      <c r="B248" s="2"/>
-      <c r="C248" s="2"/>
-    </row>
-    <row r="249" customFormat="false" ht="12.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A249" s="2"/>
-      <c r="B249" s="2"/>
-      <c r="C249" s="2"/>
-    </row>
-    <row r="250" customFormat="false" ht="12.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A250" s="2"/>
-      <c r="B250" s="2"/>
-      <c r="C250" s="2"/>
-    </row>
-    <row r="251" customFormat="false" ht="12.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A251" s="2"/>
-      <c r="B251" s="2"/>
-      <c r="C251" s="2"/>
-    </row>
-    <row r="252" customFormat="false" ht="12.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A252" s="2"/>
-      <c r="B252" s="2"/>
-      <c r="C252" s="2"/>
-    </row>
-    <row r="253" customFormat="false" ht="12.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A253" s="2"/>
-      <c r="B253" s="2"/>
-      <c r="C253" s="2"/>
-    </row>
-    <row r="254" customFormat="false" ht="12.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A254" s="2"/>
-      <c r="B254" s="2"/>
-      <c r="C254" s="2"/>
-    </row>
-    <row r="255" customFormat="false" ht="12.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A255" s="2"/>
-      <c r="B255" s="2"/>
-      <c r="C255" s="2"/>
-    </row>
-    <row r="256" customFormat="false" ht="12.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A256" s="2"/>
-      <c r="B256" s="2"/>
-      <c r="C256" s="2"/>
-    </row>
-    <row r="257" customFormat="false" ht="12.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A257" s="2"/>
-      <c r="B257" s="2"/>
-      <c r="C257" s="2"/>
-    </row>
-    <row r="258" customFormat="false" ht="12.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A258" s="2"/>
-      <c r="B258" s="2"/>
-      <c r="C258" s="2"/>
-    </row>
-    <row r="259" customFormat="false" ht="12.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A259" s="2"/>
-      <c r="B259" s="2"/>
-      <c r="C259" s="2"/>
-    </row>
-    <row r="260" customFormat="false" ht="12.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A260" s="2"/>
-      <c r="B260" s="2"/>
-      <c r="C260" s="2"/>
-    </row>
-    <row r="261" customFormat="false" ht="12.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A261" s="2"/>
-      <c r="B261" s="2"/>
-      <c r="C261" s="2"/>
-    </row>
-    <row r="262" customFormat="false" ht="12.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A262" s="2"/>
-      <c r="B262" s="2"/>
-      <c r="C262" s="2"/>
-    </row>
-    <row r="263" customFormat="false" ht="12.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A263" s="2"/>
-      <c r="B263" s="2"/>
-      <c r="C263" s="2"/>
-    </row>
-    <row r="264" customFormat="false" ht="12.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A264" s="2"/>
-      <c r="B264" s="2"/>
-      <c r="C264" s="2"/>
-    </row>
-    <row r="265" customFormat="false" ht="12.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A265" s="2"/>
-      <c r="B265" s="2"/>
-      <c r="C265" s="2"/>
-    </row>
-    <row r="266" customFormat="false" ht="12.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A266" s="2"/>
-      <c r="B266" s="2"/>
-      <c r="C266" s="2"/>
-    </row>
-    <row r="267" customFormat="false" ht="12.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A267" s="2"/>
-      <c r="B267" s="2"/>
-      <c r="C267" s="2"/>
-    </row>
-    <row r="268" customFormat="false" ht="12.8" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
-      <c r="A268" s="2"/>
-      <c r="B268" s="2"/>
-      <c r="C268" s="2"/>
-    </row>
+    <row r="1048576" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
   </sheetData>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.7875" right="0.7875" top="1.05277777777778" bottom="1.05277777777778" header="0.7875" footer="0.7875"/>

</xml_diff>

<commit_message>
Update failure Test results
</commit_message>
<xml_diff>
--- a/attendance/src/main/resources/LeaveDeductions.xlsx
+++ b/attendance/src/main/resources/LeaveDeductions.xlsx
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="639" uniqueCount="231">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="710" uniqueCount="234">
   <si>
     <t xml:space="preserve">TCID</t>
   </si>
@@ -49,6 +49,9 @@
     <t xml:space="preserve">TestDataRow</t>
   </si>
   <si>
+    <t xml:space="preserve">RunMode</t>
+  </si>
+  <si>
     <t xml:space="preserve">1</t>
   </si>
   <si>
@@ -76,6 +79,9 @@
     <t xml:space="preserve">1-32</t>
   </si>
   <si>
+    <t xml:space="preserve">no</t>
+  </si>
+  <si>
     <t xml:space="preserve">2</t>
   </si>
   <si>
@@ -263,6 +269,9 @@
   </si>
   <si>
     <t xml:space="preserve">com.darwinbox.attendance.leavedeductions.totalduration.fullday.TestForTotalDurationFullDayDeduction</t>
+  </si>
+  <si>
+    <t xml:space="preserve">yes</t>
   </si>
   <si>
     <t xml:space="preserve">22</t>
@@ -794,13 +803,17 @@
     <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="3">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
     <xf numFmtId="164" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
   </cellXfs>
@@ -820,10 +833,10 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:I71"/>
+  <dimension ref="A1:J71"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="F55" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="H59" activeCellId="0" sqref="H59:H71"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A64" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="A69" activeCellId="0" sqref="A69"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15.75" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -867,2035 +880,2248 @@
       <c r="I1" s="1" t="s">
         <v>8</v>
       </c>
+      <c r="J1" s="2" t="s">
+        <v>9</v>
+      </c>
     </row>
     <row r="2" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A2" s="0" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="B2" s="0" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="C2" s="0" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="D2" s="0" t="s">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="E2" s="0" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="F2" s="0" t="s">
-        <v>14</v>
+        <v>15</v>
       </c>
       <c r="G2" s="0" t="s">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="H2" s="0" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="I2" s="0" t="s">
-        <v>17</v>
+        <v>18</v>
+      </c>
+      <c r="J2" s="0" t="s">
+        <v>19</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A3" s="0" t="s">
-        <v>18</v>
+        <v>20</v>
       </c>
       <c r="B3" s="0" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="C3" s="0" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="D3" s="0" t="s">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="E3" s="0" t="s">
-        <v>19</v>
+        <v>21</v>
       </c>
       <c r="F3" s="0" t="s">
-        <v>20</v>
+        <v>22</v>
       </c>
       <c r="G3" s="0" t="s">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="H3" s="0" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="I3" s="0" t="s">
-        <v>17</v>
+        <v>18</v>
+      </c>
+      <c r="J3" s="0" t="s">
+        <v>19</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A4" s="0" t="s">
-        <v>21</v>
+        <v>23</v>
       </c>
       <c r="B4" s="0" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="C4" s="0" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="D4" s="0" t="s">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="E4" s="0" t="s">
-        <v>22</v>
+        <v>24</v>
       </c>
       <c r="F4" s="0" t="s">
-        <v>23</v>
+        <v>25</v>
       </c>
       <c r="G4" s="0" t="s">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="H4" s="0" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="I4" s="0" t="s">
-        <v>17</v>
+        <v>18</v>
+      </c>
+      <c r="J4" s="0" t="s">
+        <v>19</v>
       </c>
     </row>
     <row r="5" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A5" s="0" t="s">
-        <v>24</v>
+        <v>26</v>
       </c>
       <c r="B5" s="0" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="C5" s="0" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="D5" s="0" t="s">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="E5" s="0" t="s">
-        <v>25</v>
+        <v>27</v>
       </c>
       <c r="F5" s="0" t="s">
-        <v>26</v>
+        <v>28</v>
       </c>
       <c r="G5" s="0" t="s">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="H5" s="0" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="I5" s="0" t="s">
-        <v>17</v>
+        <v>18</v>
+      </c>
+      <c r="J5" s="0" t="s">
+        <v>19</v>
       </c>
     </row>
     <row r="6" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A6" s="0" t="s">
-        <v>27</v>
+        <v>29</v>
       </c>
       <c r="B6" s="0" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="C6" s="0" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="D6" s="0" t="s">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="E6" s="0" t="s">
-        <v>28</v>
+        <v>30</v>
       </c>
       <c r="F6" s="0" t="s">
-        <v>29</v>
+        <v>31</v>
       </c>
       <c r="G6" s="0" t="s">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="H6" s="0" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="I6" s="0" t="s">
-        <v>17</v>
+        <v>18</v>
+      </c>
+      <c r="J6" s="0" t="s">
+        <v>19</v>
       </c>
     </row>
     <row r="7" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A7" s="0" t="s">
-        <v>30</v>
+        <v>32</v>
       </c>
       <c r="B7" s="0" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="C7" s="0" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="D7" s="0" t="s">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="E7" s="0" t="s">
-        <v>31</v>
+        <v>33</v>
       </c>
       <c r="F7" s="0" t="s">
-        <v>32</v>
+        <v>34</v>
       </c>
       <c r="G7" s="0" t="s">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="H7" s="0" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="I7" s="0" t="s">
-        <v>17</v>
+        <v>18</v>
+      </c>
+      <c r="J7" s="0" t="s">
+        <v>19</v>
       </c>
     </row>
     <row r="8" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A8" s="0" t="s">
-        <v>33</v>
+        <v>35</v>
       </c>
       <c r="B8" s="0" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="C8" s="0" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="D8" s="0" t="s">
-        <v>34</v>
+        <v>36</v>
       </c>
       <c r="E8" s="0" t="s">
-        <v>35</v>
+        <v>37</v>
       </c>
       <c r="F8" s="0" t="s">
-        <v>36</v>
+        <v>38</v>
       </c>
       <c r="G8" s="0" t="s">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="H8" s="0" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="I8" s="0" t="s">
-        <v>17</v>
+        <v>18</v>
+      </c>
+      <c r="J8" s="0" t="s">
+        <v>19</v>
       </c>
     </row>
     <row r="9" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A9" s="0" t="s">
-        <v>37</v>
+        <v>39</v>
       </c>
       <c r="B9" s="0" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="C9" s="0" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="D9" s="0" t="s">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="E9" s="0" t="s">
-        <v>38</v>
+        <v>40</v>
       </c>
       <c r="F9" s="0" t="s">
-        <v>39</v>
+        <v>41</v>
       </c>
       <c r="G9" s="0" t="s">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="H9" s="0" t="s">
-        <v>40</v>
+        <v>42</v>
       </c>
       <c r="I9" s="0" t="s">
-        <v>17</v>
+        <v>18</v>
+      </c>
+      <c r="J9" s="0" t="s">
+        <v>19</v>
       </c>
     </row>
     <row r="10" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A10" s="0" t="s">
-        <v>41</v>
+        <v>43</v>
       </c>
       <c r="B10" s="0" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="C10" s="0" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="D10" s="0" t="s">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="E10" s="0" t="s">
+        <v>44</v>
+      </c>
+      <c r="F10" s="0" t="s">
+        <v>45</v>
+      </c>
+      <c r="G10" s="0" t="s">
+        <v>16</v>
+      </c>
+      <c r="H10" s="0" t="s">
         <v>42</v>
       </c>
-      <c r="F10" s="0" t="s">
-        <v>43</v>
-      </c>
-      <c r="G10" s="0" t="s">
-        <v>15</v>
-      </c>
-      <c r="H10" s="0" t="s">
-        <v>40</v>
-      </c>
       <c r="I10" s="0" t="s">
-        <v>17</v>
+        <v>18</v>
+      </c>
+      <c r="J10" s="0" t="s">
+        <v>19</v>
       </c>
     </row>
     <row r="11" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A11" s="0" t="s">
-        <v>44</v>
+        <v>46</v>
       </c>
       <c r="B11" s="0" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="C11" s="0" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="D11" s="0" t="s">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="E11" s="0" t="s">
-        <v>45</v>
+        <v>47</v>
       </c>
       <c r="F11" s="0" t="s">
-        <v>46</v>
+        <v>48</v>
       </c>
       <c r="G11" s="0" t="s">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="H11" s="0" t="s">
-        <v>40</v>
+        <v>42</v>
       </c>
       <c r="I11" s="0" t="s">
-        <v>17</v>
+        <v>18</v>
+      </c>
+      <c r="J11" s="0" t="s">
+        <v>19</v>
       </c>
     </row>
     <row r="12" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A12" s="0" t="s">
-        <v>47</v>
+        <v>49</v>
       </c>
       <c r="B12" s="0" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="C12" s="0" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="D12" s="0" t="s">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="E12" s="0" t="s">
-        <v>48</v>
+        <v>50</v>
       </c>
       <c r="F12" s="0" t="s">
-        <v>49</v>
+        <v>51</v>
       </c>
       <c r="G12" s="0" t="s">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="H12" s="0" t="s">
-        <v>40</v>
+        <v>42</v>
       </c>
       <c r="I12" s="0" t="s">
-        <v>17</v>
+        <v>18</v>
+      </c>
+      <c r="J12" s="0" t="s">
+        <v>19</v>
       </c>
     </row>
     <row r="13" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A13" s="0" t="s">
-        <v>50</v>
+        <v>52</v>
       </c>
       <c r="B13" s="0" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="C13" s="0" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="D13" s="0" t="s">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="E13" s="0" t="s">
-        <v>51</v>
+        <v>53</v>
       </c>
       <c r="F13" s="0" t="s">
-        <v>52</v>
+        <v>54</v>
       </c>
       <c r="G13" s="0" t="s">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="H13" s="0" t="s">
-        <v>40</v>
+        <v>42</v>
       </c>
       <c r="I13" s="0" t="s">
-        <v>17</v>
+        <v>18</v>
+      </c>
+      <c r="J13" s="0" t="s">
+        <v>19</v>
       </c>
     </row>
     <row r="14" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A14" s="0" t="s">
-        <v>53</v>
+        <v>55</v>
       </c>
       <c r="B14" s="0" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="C14" s="0" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="D14" s="0" t="s">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="E14" s="0" t="s">
-        <v>54</v>
+        <v>56</v>
       </c>
       <c r="F14" s="0" t="s">
-        <v>55</v>
+        <v>57</v>
       </c>
       <c r="G14" s="0" t="s">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="H14" s="0" t="s">
-        <v>40</v>
+        <v>42</v>
       </c>
       <c r="I14" s="0" t="s">
-        <v>17</v>
+        <v>18</v>
+      </c>
+      <c r="J14" s="0" t="s">
+        <v>19</v>
       </c>
     </row>
     <row r="15" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A15" s="0" t="s">
-        <v>56</v>
+        <v>58</v>
       </c>
       <c r="B15" s="0" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="C15" s="0" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="D15" s="0" t="s">
-        <v>34</v>
+        <v>36</v>
       </c>
       <c r="E15" s="0" t="s">
-        <v>57</v>
+        <v>59</v>
       </c>
       <c r="F15" s="0" t="s">
-        <v>58</v>
+        <v>60</v>
       </c>
       <c r="G15" s="0" t="s">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="H15" s="0" t="s">
-        <v>40</v>
+        <v>42</v>
       </c>
       <c r="I15" s="0" t="s">
-        <v>17</v>
+        <v>18</v>
+      </c>
+      <c r="J15" s="0" t="s">
+        <v>19</v>
       </c>
     </row>
     <row r="16" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A16" s="0" t="s">
-        <v>59</v>
+        <v>61</v>
       </c>
       <c r="B16" s="0" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="C16" s="0" t="s">
-        <v>60</v>
+        <v>62</v>
       </c>
       <c r="D16" s="0" t="s">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="E16" s="0" t="s">
-        <v>61</v>
+        <v>63</v>
       </c>
       <c r="F16" s="0" t="s">
+        <v>64</v>
+      </c>
+      <c r="G16" s="0" t="s">
+        <v>16</v>
+      </c>
+      <c r="H16" s="0" t="s">
         <v>62</v>
       </c>
-      <c r="G16" s="0" t="s">
-        <v>15</v>
-      </c>
-      <c r="H16" s="0" t="s">
-        <v>60</v>
-      </c>
       <c r="I16" s="0" t="s">
-        <v>17</v>
+        <v>18</v>
+      </c>
+      <c r="J16" s="0" t="s">
+        <v>19</v>
       </c>
     </row>
     <row r="17" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A17" s="0" t="s">
-        <v>63</v>
+        <v>65</v>
       </c>
       <c r="B17" s="0" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="C17" s="0" t="s">
-        <v>60</v>
+        <v>62</v>
       </c>
       <c r="D17" s="0" t="s">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="E17" s="0" t="s">
-        <v>64</v>
+        <v>66</v>
       </c>
       <c r="F17" s="0" t="s">
-        <v>65</v>
+        <v>67</v>
       </c>
       <c r="G17" s="0" t="s">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="H17" s="0" t="s">
-        <v>60</v>
+        <v>62</v>
       </c>
       <c r="I17" s="0" t="s">
-        <v>17</v>
+        <v>18</v>
+      </c>
+      <c r="J17" s="0" t="s">
+        <v>19</v>
       </c>
     </row>
     <row r="18" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A18" s="0" t="s">
-        <v>66</v>
+        <v>68</v>
       </c>
       <c r="B18" s="0" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="C18" s="0" t="s">
-        <v>60</v>
+        <v>62</v>
       </c>
       <c r="D18" s="0" t="s">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="E18" s="0" t="s">
-        <v>67</v>
+        <v>69</v>
       </c>
       <c r="F18" s="0" t="s">
-        <v>68</v>
+        <v>70</v>
       </c>
       <c r="G18" s="0" t="s">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="H18" s="0" t="s">
-        <v>60</v>
+        <v>62</v>
       </c>
       <c r="I18" s="0" t="s">
-        <v>17</v>
+        <v>18</v>
+      </c>
+      <c r="J18" s="0" t="s">
+        <v>19</v>
       </c>
     </row>
     <row r="19" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A19" s="0" t="s">
-        <v>69</v>
+        <v>71</v>
       </c>
       <c r="B19" s="0" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="C19" s="0" t="s">
-        <v>60</v>
+        <v>62</v>
       </c>
       <c r="D19" s="0" t="s">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="E19" s="0" t="s">
-        <v>70</v>
+        <v>72</v>
       </c>
       <c r="F19" s="0" t="s">
-        <v>71</v>
+        <v>73</v>
       </c>
       <c r="G19" s="0" t="s">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="H19" s="0" t="s">
-        <v>60</v>
+        <v>62</v>
       </c>
       <c r="I19" s="0" t="s">
-        <v>17</v>
+        <v>18</v>
+      </c>
+      <c r="J19" s="0" t="s">
+        <v>19</v>
       </c>
     </row>
     <row r="20" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A20" s="0" t="s">
-        <v>72</v>
+        <v>74</v>
       </c>
       <c r="B20" s="0" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="C20" s="0" t="s">
-        <v>60</v>
+        <v>62</v>
       </c>
       <c r="D20" s="0" t="s">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="E20" s="0" t="s">
-        <v>73</v>
+        <v>75</v>
       </c>
       <c r="F20" s="0" t="s">
-        <v>74</v>
+        <v>76</v>
       </c>
       <c r="G20" s="0" t="s">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="H20" s="0" t="s">
-        <v>60</v>
+        <v>62</v>
       </c>
       <c r="I20" s="0" t="s">
-        <v>17</v>
+        <v>18</v>
+      </c>
+      <c r="J20" s="0" t="s">
+        <v>19</v>
       </c>
     </row>
     <row r="21" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A21" s="0" t="s">
-        <v>75</v>
+        <v>77</v>
       </c>
       <c r="B21" s="0" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="C21" s="0" t="s">
-        <v>60</v>
+        <v>62</v>
       </c>
       <c r="D21" s="0" t="s">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="E21" s="0" t="s">
-        <v>76</v>
+        <v>78</v>
       </c>
       <c r="F21" s="0" t="s">
-        <v>77</v>
+        <v>79</v>
       </c>
       <c r="G21" s="0" t="s">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="H21" s="0" t="s">
-        <v>60</v>
+        <v>62</v>
       </c>
       <c r="I21" s="0" t="s">
-        <v>17</v>
+        <v>18</v>
+      </c>
+      <c r="J21" s="0" t="s">
+        <v>19</v>
       </c>
     </row>
     <row r="22" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A22" s="0" t="s">
-        <v>78</v>
+        <v>80</v>
       </c>
       <c r="B22" s="0" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="C22" s="0" t="s">
-        <v>60</v>
+        <v>62</v>
       </c>
       <c r="D22" s="0" t="s">
-        <v>34</v>
+        <v>36</v>
       </c>
       <c r="E22" s="0" t="s">
-        <v>79</v>
+        <v>81</v>
       </c>
       <c r="F22" s="0" t="s">
-        <v>80</v>
+        <v>82</v>
       </c>
       <c r="G22" s="0" t="s">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="H22" s="0" t="s">
-        <v>60</v>
+        <v>62</v>
       </c>
       <c r="I22" s="0" t="s">
-        <v>17</v>
+        <v>18</v>
+      </c>
+      <c r="J22" s="0" t="s">
+        <v>83</v>
       </c>
     </row>
     <row r="23" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A23" s="0" t="s">
-        <v>81</v>
+        <v>84</v>
       </c>
       <c r="B23" s="0" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="C23" s="0" t="s">
-        <v>60</v>
+        <v>62</v>
       </c>
       <c r="D23" s="0" t="s">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="E23" s="0" t="s">
-        <v>82</v>
+        <v>85</v>
       </c>
       <c r="F23" s="0" t="s">
-        <v>83</v>
+        <v>86</v>
       </c>
       <c r="G23" s="0" t="s">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="H23" s="0" t="s">
-        <v>60</v>
+        <v>62</v>
       </c>
       <c r="I23" s="0" t="s">
-        <v>17</v>
+        <v>18</v>
+      </c>
+      <c r="J23" s="0" t="s">
+        <v>19</v>
       </c>
     </row>
     <row r="24" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A24" s="0" t="s">
-        <v>84</v>
+        <v>87</v>
       </c>
       <c r="B24" s="0" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="C24" s="0" t="s">
-        <v>60</v>
+        <v>62</v>
       </c>
       <c r="D24" s="0" t="s">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="E24" s="0" t="s">
-        <v>85</v>
+        <v>88</v>
       </c>
       <c r="F24" s="0" t="s">
-        <v>86</v>
+        <v>89</v>
       </c>
       <c r="G24" s="0" t="s">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="H24" s="0" t="s">
-        <v>60</v>
+        <v>62</v>
       </c>
       <c r="I24" s="0" t="s">
-        <v>17</v>
+        <v>18</v>
+      </c>
+      <c r="J24" s="0" t="s">
+        <v>19</v>
       </c>
     </row>
     <row r="25" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A25" s="0" t="s">
-        <v>87</v>
+        <v>90</v>
       </c>
       <c r="B25" s="0" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="C25" s="0" t="s">
-        <v>60</v>
+        <v>62</v>
       </c>
       <c r="D25" s="0" t="s">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="E25" s="0" t="s">
-        <v>88</v>
+        <v>91</v>
       </c>
       <c r="F25" s="0" t="s">
-        <v>89</v>
+        <v>92</v>
       </c>
       <c r="G25" s="0" t="s">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="H25" s="0" t="s">
-        <v>60</v>
+        <v>62</v>
       </c>
       <c r="I25" s="0" t="s">
-        <v>17</v>
+        <v>18</v>
+      </c>
+      <c r="J25" s="0" t="s">
+        <v>19</v>
       </c>
     </row>
     <row r="26" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A26" s="0" t="s">
-        <v>90</v>
+        <v>93</v>
       </c>
       <c r="B26" s="0" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="C26" s="0" t="s">
-        <v>60</v>
+        <v>62</v>
       </c>
       <c r="D26" s="0" t="s">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="E26" s="0" t="s">
-        <v>91</v>
+        <v>94</v>
       </c>
       <c r="F26" s="0" t="s">
-        <v>92</v>
+        <v>95</v>
       </c>
       <c r="G26" s="0" t="s">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="H26" s="0" t="s">
-        <v>60</v>
+        <v>62</v>
       </c>
       <c r="I26" s="0" t="s">
-        <v>17</v>
+        <v>18</v>
+      </c>
+      <c r="J26" s="0" t="s">
+        <v>19</v>
       </c>
     </row>
     <row r="27" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A27" s="0" t="s">
-        <v>93</v>
+        <v>96</v>
       </c>
       <c r="B27" s="0" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="C27" s="0" t="s">
-        <v>60</v>
+        <v>62</v>
       </c>
       <c r="D27" s="0" t="s">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="E27" s="0" t="s">
-        <v>94</v>
+        <v>97</v>
       </c>
       <c r="F27" s="0" t="s">
-        <v>95</v>
+        <v>98</v>
       </c>
       <c r="G27" s="0" t="s">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="H27" s="0" t="s">
-        <v>60</v>
+        <v>62</v>
       </c>
       <c r="I27" s="0" t="s">
-        <v>17</v>
+        <v>18</v>
+      </c>
+      <c r="J27" s="0" t="s">
+        <v>19</v>
       </c>
     </row>
     <row r="28" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A28" s="0" t="s">
-        <v>96</v>
+        <v>99</v>
       </c>
       <c r="B28" s="0" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="C28" s="0" t="s">
-        <v>60</v>
+        <v>62</v>
       </c>
       <c r="D28" s="0" t="s">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="E28" s="0" t="s">
-        <v>97</v>
+        <v>100</v>
       </c>
       <c r="F28" s="0" t="s">
-        <v>98</v>
+        <v>101</v>
       </c>
       <c r="G28" s="0" t="s">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="H28" s="0" t="s">
-        <v>60</v>
+        <v>62</v>
       </c>
       <c r="I28" s="0" t="s">
-        <v>17</v>
+        <v>18</v>
+      </c>
+      <c r="J28" s="0" t="s">
+        <v>19</v>
       </c>
     </row>
     <row r="29" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A29" s="0" t="s">
-        <v>99</v>
+        <v>102</v>
       </c>
       <c r="B29" s="0" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="C29" s="0" t="s">
-        <v>60</v>
+        <v>62</v>
       </c>
       <c r="D29" s="0" t="s">
-        <v>34</v>
+        <v>36</v>
       </c>
       <c r="E29" s="0" t="s">
-        <v>100</v>
+        <v>103</v>
       </c>
       <c r="F29" s="0" t="s">
-        <v>101</v>
+        <v>104</v>
       </c>
       <c r="G29" s="0" t="s">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="H29" s="0" t="s">
-        <v>60</v>
+        <v>62</v>
       </c>
       <c r="I29" s="0" t="s">
-        <v>17</v>
+        <v>18</v>
+      </c>
+      <c r="J29" s="0" t="s">
+        <v>83</v>
       </c>
     </row>
     <row r="30" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A30" s="0" t="s">
-        <v>102</v>
+        <v>105</v>
       </c>
       <c r="B30" s="0" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="C30" s="0" t="s">
-        <v>103</v>
+        <v>106</v>
       </c>
       <c r="D30" s="0" t="s">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="E30" s="0" t="s">
-        <v>104</v>
+        <v>107</v>
       </c>
       <c r="F30" s="0" t="s">
-        <v>105</v>
+        <v>108</v>
       </c>
       <c r="G30" s="0" t="s">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="H30" s="0" t="s">
-        <v>103</v>
+        <v>106</v>
       </c>
       <c r="I30" s="0" t="s">
-        <v>17</v>
+        <v>18</v>
+      </c>
+      <c r="J30" s="0" t="s">
+        <v>19</v>
       </c>
     </row>
     <row r="31" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A31" s="0" t="s">
+        <v>109</v>
+      </c>
+      <c r="B31" s="0" t="s">
+        <v>11</v>
+      </c>
+      <c r="C31" s="0" t="s">
         <v>106</v>
       </c>
-      <c r="B31" s="0" t="s">
-        <v>10</v>
-      </c>
-      <c r="C31" s="0" t="s">
-        <v>103</v>
-      </c>
       <c r="D31" s="0" t="s">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="E31" s="0" t="s">
-        <v>107</v>
+        <v>110</v>
       </c>
       <c r="F31" s="0" t="s">
-        <v>108</v>
+        <v>111</v>
       </c>
       <c r="G31" s="0" t="s">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="H31" s="0" t="s">
-        <v>103</v>
+        <v>106</v>
       </c>
       <c r="I31" s="0" t="s">
-        <v>17</v>
+        <v>18</v>
+      </c>
+      <c r="J31" s="0" t="s">
+        <v>19</v>
       </c>
     </row>
     <row r="32" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A32" s="0" t="s">
-        <v>109</v>
+        <v>112</v>
       </c>
       <c r="B32" s="0" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="C32" s="0" t="s">
-        <v>103</v>
+        <v>106</v>
       </c>
       <c r="D32" s="0" t="s">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="E32" s="0" t="s">
-        <v>110</v>
+        <v>113</v>
       </c>
       <c r="F32" s="0" t="s">
-        <v>111</v>
+        <v>114</v>
       </c>
       <c r="G32" s="0" t="s">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="H32" s="0" t="s">
-        <v>103</v>
+        <v>106</v>
       </c>
       <c r="I32" s="0" t="s">
-        <v>17</v>
+        <v>18</v>
+      </c>
+      <c r="J32" s="0" t="s">
+        <v>19</v>
       </c>
     </row>
     <row r="33" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A33" s="0" t="s">
-        <v>112</v>
+        <v>115</v>
       </c>
       <c r="B33" s="0" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="C33" s="0" t="s">
-        <v>103</v>
+        <v>106</v>
       </c>
       <c r="D33" s="0" t="s">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="E33" s="0" t="s">
-        <v>113</v>
+        <v>116</v>
       </c>
       <c r="F33" s="0" t="s">
-        <v>114</v>
+        <v>117</v>
       </c>
       <c r="G33" s="0" t="s">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="H33" s="0" t="s">
-        <v>103</v>
+        <v>106</v>
       </c>
       <c r="I33" s="0" t="s">
-        <v>17</v>
+        <v>18</v>
+      </c>
+      <c r="J33" s="0" t="s">
+        <v>19</v>
       </c>
     </row>
     <row r="34" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A34" s="0" t="s">
-        <v>115</v>
+        <v>118</v>
       </c>
       <c r="B34" s="0" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="C34" s="0" t="s">
-        <v>103</v>
+        <v>106</v>
       </c>
       <c r="D34" s="0" t="s">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="E34" s="0" t="s">
-        <v>116</v>
+        <v>119</v>
       </c>
       <c r="F34" s="0" t="s">
-        <v>117</v>
+        <v>120</v>
       </c>
       <c r="G34" s="0" t="s">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="H34" s="0" t="s">
-        <v>103</v>
+        <v>106</v>
       </c>
       <c r="I34" s="0" t="s">
-        <v>17</v>
+        <v>18</v>
+      </c>
+      <c r="J34" s="0" t="s">
+        <v>19</v>
       </c>
     </row>
     <row r="35" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A35" s="0" t="s">
-        <v>118</v>
+        <v>121</v>
       </c>
       <c r="B35" s="0" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="C35" s="0" t="s">
-        <v>103</v>
+        <v>106</v>
       </c>
       <c r="D35" s="0" t="s">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="E35" s="0" t="s">
-        <v>119</v>
+        <v>122</v>
       </c>
       <c r="F35" s="0" t="s">
-        <v>120</v>
+        <v>123</v>
       </c>
       <c r="G35" s="0" t="s">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="H35" s="0" t="s">
-        <v>103</v>
+        <v>106</v>
       </c>
       <c r="I35" s="0" t="s">
-        <v>17</v>
+        <v>18</v>
+      </c>
+      <c r="J35" s="0" t="s">
+        <v>19</v>
       </c>
     </row>
     <row r="36" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A36" s="0" t="s">
-        <v>121</v>
+        <v>124</v>
       </c>
       <c r="B36" s="0" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="C36" s="0" t="s">
-        <v>103</v>
+        <v>106</v>
       </c>
       <c r="D36" s="0" t="s">
-        <v>34</v>
+        <v>36</v>
       </c>
       <c r="E36" s="0" t="s">
-        <v>122</v>
+        <v>125</v>
       </c>
       <c r="F36" s="0" t="s">
-        <v>123</v>
+        <v>126</v>
       </c>
       <c r="G36" s="0" t="s">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="H36" s="0" t="s">
-        <v>103</v>
+        <v>106</v>
       </c>
       <c r="I36" s="0" t="s">
-        <v>17</v>
+        <v>18</v>
+      </c>
+      <c r="J36" s="0" t="s">
+        <v>83</v>
       </c>
     </row>
     <row r="37" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A37" s="0" t="s">
-        <v>124</v>
+        <v>127</v>
       </c>
       <c r="B37" s="0" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="C37" s="0" t="s">
-        <v>103</v>
+        <v>106</v>
       </c>
       <c r="D37" s="0" t="s">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="E37" s="0" t="s">
-        <v>125</v>
+        <v>128</v>
       </c>
       <c r="F37" s="0" t="s">
-        <v>126</v>
+        <v>129</v>
       </c>
       <c r="G37" s="0" t="s">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="H37" s="0" t="s">
-        <v>103</v>
+        <v>106</v>
       </c>
       <c r="I37" s="0" t="s">
-        <v>17</v>
+        <v>18</v>
+      </c>
+      <c r="J37" s="0" t="s">
+        <v>19</v>
       </c>
     </row>
     <row r="38" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A38" s="0" t="s">
-        <v>127</v>
+        <v>130</v>
       </c>
       <c r="B38" s="0" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="C38" s="0" t="s">
-        <v>103</v>
+        <v>106</v>
       </c>
       <c r="D38" s="0" t="s">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="E38" s="0" t="s">
-        <v>128</v>
+        <v>131</v>
       </c>
       <c r="F38" s="0" t="s">
-        <v>129</v>
+        <v>132</v>
       </c>
       <c r="G38" s="0" t="s">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="H38" s="0" t="s">
-        <v>103</v>
+        <v>106</v>
       </c>
       <c r="I38" s="0" t="s">
-        <v>17</v>
+        <v>18</v>
+      </c>
+      <c r="J38" s="0" t="s">
+        <v>19</v>
       </c>
     </row>
     <row r="39" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A39" s="0" t="s">
-        <v>130</v>
+        <v>133</v>
       </c>
       <c r="B39" s="0" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="C39" s="0" t="s">
-        <v>103</v>
+        <v>106</v>
       </c>
       <c r="D39" s="0" t="s">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="E39" s="0" t="s">
-        <v>131</v>
+        <v>134</v>
       </c>
       <c r="F39" s="0" t="s">
-        <v>132</v>
+        <v>135</v>
       </c>
       <c r="G39" s="0" t="s">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="H39" s="0" t="s">
-        <v>103</v>
+        <v>106</v>
       </c>
       <c r="I39" s="0" t="s">
-        <v>17</v>
+        <v>18</v>
+      </c>
+      <c r="J39" s="0" t="s">
+        <v>19</v>
       </c>
     </row>
     <row r="40" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A40" s="0" t="s">
-        <v>133</v>
+        <v>136</v>
       </c>
       <c r="B40" s="0" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="C40" s="0" t="s">
-        <v>103</v>
+        <v>106</v>
       </c>
       <c r="D40" s="0" t="s">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="E40" s="0" t="s">
-        <v>134</v>
+        <v>137</v>
       </c>
       <c r="F40" s="0" t="s">
-        <v>135</v>
+        <v>138</v>
       </c>
       <c r="G40" s="0" t="s">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="H40" s="0" t="s">
-        <v>103</v>
+        <v>106</v>
       </c>
       <c r="I40" s="0" t="s">
-        <v>17</v>
+        <v>18</v>
+      </c>
+      <c r="J40" s="0" t="s">
+        <v>19</v>
       </c>
     </row>
     <row r="41" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A41" s="0" t="s">
-        <v>136</v>
+        <v>139</v>
       </c>
       <c r="B41" s="0" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="C41" s="0" t="s">
-        <v>103</v>
+        <v>106</v>
       </c>
       <c r="D41" s="0" t="s">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="E41" s="0" t="s">
-        <v>137</v>
+        <v>140</v>
       </c>
       <c r="F41" s="0" t="s">
-        <v>138</v>
+        <v>141</v>
       </c>
       <c r="G41" s="0" t="s">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="H41" s="0" t="s">
-        <v>103</v>
+        <v>106</v>
       </c>
       <c r="I41" s="0" t="s">
-        <v>17</v>
+        <v>18</v>
+      </c>
+      <c r="J41" s="0" t="s">
+        <v>19</v>
       </c>
     </row>
     <row r="42" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A42" s="0" t="s">
-        <v>139</v>
+        <v>142</v>
       </c>
       <c r="B42" s="0" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="C42" s="0" t="s">
-        <v>103</v>
+        <v>106</v>
       </c>
       <c r="D42" s="0" t="s">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="E42" s="0" t="s">
-        <v>140</v>
+        <v>143</v>
       </c>
       <c r="F42" s="0" t="s">
-        <v>141</v>
+        <v>144</v>
       </c>
       <c r="G42" s="0" t="s">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="H42" s="0" t="s">
-        <v>103</v>
+        <v>106</v>
       </c>
       <c r="I42" s="0" t="s">
-        <v>17</v>
+        <v>18</v>
+      </c>
+      <c r="J42" s="0" t="s">
+        <v>19</v>
       </c>
     </row>
     <row r="43" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A43" s="0" t="s">
-        <v>142</v>
+        <v>145</v>
       </c>
       <c r="B43" s="0" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="C43" s="0" t="s">
-        <v>103</v>
+        <v>106</v>
       </c>
       <c r="D43" s="0" t="s">
-        <v>34</v>
+        <v>36</v>
       </c>
       <c r="E43" s="0" t="s">
-        <v>143</v>
+        <v>146</v>
       </c>
       <c r="F43" s="0" t="s">
-        <v>144</v>
+        <v>147</v>
       </c>
       <c r="G43" s="0" t="s">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="H43" s="0" t="s">
-        <v>103</v>
+        <v>106</v>
       </c>
       <c r="I43" s="0" t="s">
-        <v>17</v>
+        <v>18</v>
+      </c>
+      <c r="J43" s="0" t="s">
+        <v>83</v>
       </c>
     </row>
     <row r="44" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A44" s="0" t="s">
-        <v>145</v>
+        <v>148</v>
       </c>
       <c r="B44" s="0" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="C44" s="0" t="s">
-        <v>146</v>
+        <v>149</v>
       </c>
       <c r="D44" s="0" t="s">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="E44" s="0" t="s">
-        <v>147</v>
+        <v>150</v>
       </c>
       <c r="F44" s="0" t="s">
-        <v>148</v>
+        <v>151</v>
       </c>
       <c r="G44" s="0" t="s">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="H44" s="0" t="s">
-        <v>146</v>
+        <v>149</v>
       </c>
       <c r="I44" s="0" t="s">
-        <v>17</v>
+        <v>18</v>
+      </c>
+      <c r="J44" s="0" t="s">
+        <v>19</v>
       </c>
     </row>
     <row r="45" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A45" s="0" t="s">
+        <v>152</v>
+      </c>
+      <c r="B45" s="0" t="s">
+        <v>11</v>
+      </c>
+      <c r="C45" s="0" t="s">
         <v>149</v>
       </c>
-      <c r="B45" s="0" t="s">
-        <v>10</v>
-      </c>
-      <c r="C45" s="0" t="s">
-        <v>146</v>
-      </c>
       <c r="D45" s="0" t="s">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="E45" s="0" t="s">
-        <v>150</v>
+        <v>153</v>
       </c>
       <c r="F45" s="0" t="s">
-        <v>151</v>
+        <v>154</v>
       </c>
       <c r="G45" s="0" t="s">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="H45" s="0" t="s">
-        <v>146</v>
+        <v>149</v>
       </c>
       <c r="I45" s="0" t="s">
-        <v>17</v>
+        <v>18</v>
+      </c>
+      <c r="J45" s="0" t="s">
+        <v>19</v>
       </c>
     </row>
     <row r="46" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A46" s="0" t="s">
-        <v>152</v>
+        <v>155</v>
       </c>
       <c r="B46" s="0" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="C46" s="0" t="s">
-        <v>146</v>
+        <v>149</v>
       </c>
       <c r="D46" s="0" t="s">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="E46" s="0" t="s">
-        <v>153</v>
+        <v>156</v>
       </c>
       <c r="F46" s="0" t="s">
-        <v>154</v>
+        <v>157</v>
       </c>
       <c r="G46" s="0" t="s">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="H46" s="0" t="s">
-        <v>146</v>
+        <v>149</v>
       </c>
       <c r="I46" s="0" t="s">
-        <v>17</v>
+        <v>18</v>
+      </c>
+      <c r="J46" s="0" t="s">
+        <v>19</v>
       </c>
     </row>
     <row r="47" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A47" s="0" t="s">
-        <v>155</v>
+        <v>158</v>
       </c>
       <c r="B47" s="0" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="C47" s="0" t="s">
-        <v>146</v>
+        <v>149</v>
       </c>
       <c r="D47" s="0" t="s">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="E47" s="0" t="s">
-        <v>156</v>
+        <v>159</v>
       </c>
       <c r="F47" s="0" t="s">
-        <v>157</v>
+        <v>160</v>
       </c>
       <c r="G47" s="0" t="s">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="H47" s="0" t="s">
-        <v>146</v>
+        <v>149</v>
       </c>
       <c r="I47" s="0" t="s">
-        <v>17</v>
+        <v>18</v>
+      </c>
+      <c r="J47" s="0" t="s">
+        <v>19</v>
       </c>
     </row>
     <row r="48" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A48" s="0" t="s">
-        <v>158</v>
+        <v>161</v>
       </c>
       <c r="B48" s="0" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="C48" s="0" t="s">
-        <v>146</v>
+        <v>149</v>
       </c>
       <c r="D48" s="0" t="s">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="E48" s="0" t="s">
-        <v>159</v>
+        <v>162</v>
       </c>
       <c r="F48" s="0" t="s">
-        <v>160</v>
+        <v>163</v>
       </c>
       <c r="G48" s="0" t="s">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="H48" s="0" t="s">
-        <v>146</v>
+        <v>149</v>
       </c>
       <c r="I48" s="0" t="s">
-        <v>17</v>
+        <v>18</v>
+      </c>
+      <c r="J48" s="0" t="s">
+        <v>19</v>
       </c>
     </row>
     <row r="49" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A49" s="0" t="s">
-        <v>161</v>
+        <v>164</v>
       </c>
       <c r="B49" s="0" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="C49" s="0" t="s">
-        <v>146</v>
+        <v>149</v>
       </c>
       <c r="D49" s="0" t="s">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="E49" s="0" t="s">
-        <v>162</v>
+        <v>165</v>
       </c>
       <c r="F49" s="0" t="s">
-        <v>163</v>
+        <v>166</v>
       </c>
       <c r="G49" s="0" t="s">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="H49" s="0" t="s">
-        <v>146</v>
+        <v>149</v>
       </c>
       <c r="I49" s="0" t="s">
-        <v>17</v>
+        <v>18</v>
+      </c>
+      <c r="J49" s="0" t="s">
+        <v>19</v>
       </c>
     </row>
     <row r="50" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A50" s="0" t="s">
-        <v>164</v>
+        <v>167</v>
       </c>
       <c r="B50" s="0" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="C50" s="0" t="s">
-        <v>146</v>
+        <v>149</v>
       </c>
       <c r="D50" s="0" t="s">
-        <v>34</v>
+        <v>36</v>
       </c>
       <c r="E50" s="0" t="s">
-        <v>165</v>
+        <v>168</v>
       </c>
       <c r="F50" s="0" t="s">
-        <v>166</v>
+        <v>169</v>
       </c>
       <c r="G50" s="0" t="s">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="H50" s="0" t="s">
-        <v>146</v>
+        <v>149</v>
       </c>
       <c r="I50" s="0" t="s">
-        <v>17</v>
+        <v>18</v>
+      </c>
+      <c r="J50" s="0" t="s">
+        <v>83</v>
       </c>
     </row>
     <row r="51" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A51" s="0" t="s">
-        <v>167</v>
+        <v>170</v>
       </c>
       <c r="B51" s="0" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="C51" s="0" t="s">
-        <v>146</v>
+        <v>149</v>
       </c>
       <c r="D51" s="0" t="s">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="E51" s="0" t="s">
-        <v>168</v>
+        <v>171</v>
       </c>
       <c r="F51" s="0" t="s">
-        <v>169</v>
+        <v>172</v>
       </c>
       <c r="G51" s="0" t="s">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="H51" s="0" t="s">
-        <v>146</v>
+        <v>149</v>
       </c>
       <c r="I51" s="0" t="s">
-        <v>17</v>
+        <v>18</v>
+      </c>
+      <c r="J51" s="0" t="s">
+        <v>19</v>
       </c>
     </row>
     <row r="52" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A52" s="0" t="s">
-        <v>170</v>
+        <v>173</v>
       </c>
       <c r="B52" s="0" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="C52" s="0" t="s">
-        <v>146</v>
+        <v>149</v>
       </c>
       <c r="D52" s="0" t="s">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="E52" s="0" t="s">
-        <v>171</v>
+        <v>174</v>
       </c>
       <c r="F52" s="0" t="s">
-        <v>172</v>
+        <v>175</v>
       </c>
       <c r="G52" s="0" t="s">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="H52" s="0" t="s">
-        <v>146</v>
+        <v>149</v>
       </c>
       <c r="I52" s="0" t="s">
-        <v>17</v>
+        <v>18</v>
+      </c>
+      <c r="J52" s="0" t="s">
+        <v>19</v>
       </c>
     </row>
     <row r="53" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A53" s="0" t="s">
-        <v>173</v>
+        <v>176</v>
       </c>
       <c r="B53" s="0" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="C53" s="0" t="s">
-        <v>146</v>
+        <v>149</v>
       </c>
       <c r="D53" s="0" t="s">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="E53" s="0" t="s">
-        <v>174</v>
+        <v>177</v>
       </c>
       <c r="F53" s="0" t="s">
-        <v>175</v>
+        <v>178</v>
       </c>
       <c r="G53" s="0" t="s">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="H53" s="0" t="s">
-        <v>146</v>
+        <v>149</v>
       </c>
       <c r="I53" s="0" t="s">
-        <v>17</v>
+        <v>18</v>
+      </c>
+      <c r="J53" s="0" t="s">
+        <v>19</v>
       </c>
     </row>
     <row r="54" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A54" s="0" t="s">
-        <v>176</v>
+        <v>179</v>
       </c>
       <c r="B54" s="0" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="C54" s="0" t="s">
-        <v>146</v>
+        <v>149</v>
       </c>
       <c r="D54" s="0" t="s">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="E54" s="0" t="s">
-        <v>177</v>
+        <v>180</v>
       </c>
       <c r="F54" s="0" t="s">
-        <v>178</v>
+        <v>181</v>
       </c>
       <c r="G54" s="0" t="s">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="H54" s="0" t="s">
-        <v>146</v>
+        <v>149</v>
       </c>
       <c r="I54" s="0" t="s">
-        <v>17</v>
+        <v>18</v>
+      </c>
+      <c r="J54" s="0" t="s">
+        <v>19</v>
       </c>
     </row>
     <row r="55" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A55" s="0" t="s">
-        <v>179</v>
+        <v>182</v>
       </c>
       <c r="B55" s="0" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="C55" s="0" t="s">
-        <v>146</v>
+        <v>149</v>
       </c>
       <c r="D55" s="0" t="s">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="E55" s="0" t="s">
-        <v>180</v>
+        <v>183</v>
       </c>
       <c r="F55" s="0" t="s">
-        <v>181</v>
+        <v>184</v>
       </c>
       <c r="G55" s="0" t="s">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="H55" s="0" t="s">
-        <v>146</v>
+        <v>149</v>
       </c>
       <c r="I55" s="0" t="s">
-        <v>17</v>
+        <v>18</v>
+      </c>
+      <c r="J55" s="0" t="s">
+        <v>19</v>
       </c>
     </row>
     <row r="56" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A56" s="0" t="s">
-        <v>182</v>
+        <v>185</v>
       </c>
       <c r="B56" s="0" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="C56" s="0" t="s">
-        <v>146</v>
+        <v>149</v>
       </c>
       <c r="D56" s="0" t="s">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="E56" s="0" t="s">
-        <v>183</v>
+        <v>186</v>
       </c>
       <c r="F56" s="0" t="s">
-        <v>184</v>
+        <v>187</v>
       </c>
       <c r="G56" s="0" t="s">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="H56" s="0" t="s">
-        <v>146</v>
+        <v>149</v>
       </c>
       <c r="I56" s="0" t="s">
-        <v>17</v>
+        <v>18</v>
+      </c>
+      <c r="J56" s="0" t="s">
+        <v>19</v>
       </c>
     </row>
     <row r="57" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A57" s="0" t="s">
-        <v>185</v>
+        <v>188</v>
       </c>
       <c r="B57" s="0" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="C57" s="0" t="s">
-        <v>146</v>
+        <v>149</v>
       </c>
       <c r="D57" s="0" t="s">
-        <v>34</v>
+        <v>36</v>
       </c>
       <c r="E57" s="0" t="s">
-        <v>186</v>
+        <v>189</v>
       </c>
       <c r="F57" s="0" t="s">
-        <v>187</v>
+        <v>190</v>
       </c>
       <c r="G57" s="0" t="s">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="H57" s="0" t="s">
-        <v>146</v>
+        <v>149</v>
       </c>
       <c r="I57" s="0" t="s">
-        <v>17</v>
+        <v>18</v>
+      </c>
+      <c r="J57" s="0" t="s">
+        <v>83</v>
       </c>
     </row>
     <row r="58" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A58" s="0" t="s">
-        <v>188</v>
+        <v>191</v>
       </c>
       <c r="B58" s="0" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="C58" s="0" t="s">
-        <v>189</v>
+        <v>192</v>
       </c>
       <c r="D58" s="0" t="s">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="E58" s="0" t="s">
-        <v>190</v>
+        <v>193</v>
       </c>
       <c r="F58" s="0" t="s">
-        <v>191</v>
+        <v>194</v>
       </c>
       <c r="G58" s="0" t="s">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="H58" s="0" t="s">
-        <v>189</v>
+        <v>192</v>
       </c>
       <c r="I58" s="0" t="s">
-        <v>17</v>
+        <v>18</v>
+      </c>
+      <c r="J58" s="0" t="s">
+        <v>19</v>
       </c>
     </row>
     <row r="59" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A59" s="0" t="s">
+        <v>195</v>
+      </c>
+      <c r="B59" s="0" t="s">
+        <v>11</v>
+      </c>
+      <c r="C59" s="0" t="s">
         <v>192</v>
       </c>
-      <c r="B59" s="0" t="s">
-        <v>10</v>
-      </c>
-      <c r="C59" s="0" t="s">
-        <v>189</v>
-      </c>
       <c r="D59" s="0" t="s">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="E59" s="0" t="s">
-        <v>193</v>
+        <v>196</v>
       </c>
       <c r="F59" s="0" t="s">
-        <v>194</v>
+        <v>197</v>
       </c>
       <c r="G59" s="0" t="s">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="H59" s="0" t="s">
-        <v>189</v>
+        <v>192</v>
       </c>
       <c r="I59" s="0" t="s">
-        <v>17</v>
+        <v>18</v>
+      </c>
+      <c r="J59" s="0" t="s">
+        <v>19</v>
       </c>
     </row>
     <row r="60" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A60" s="0" t="s">
-        <v>195</v>
+        <v>198</v>
       </c>
       <c r="B60" s="0" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="C60" s="0" t="s">
-        <v>189</v>
+        <v>192</v>
       </c>
       <c r="D60" s="0" t="s">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="E60" s="0" t="s">
-        <v>196</v>
+        <v>199</v>
       </c>
       <c r="F60" s="0" t="s">
-        <v>197</v>
+        <v>200</v>
       </c>
       <c r="G60" s="0" t="s">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="H60" s="0" t="s">
-        <v>189</v>
+        <v>192</v>
       </c>
       <c r="I60" s="0" t="s">
-        <v>17</v>
+        <v>18</v>
+      </c>
+      <c r="J60" s="0" t="s">
+        <v>19</v>
       </c>
     </row>
     <row r="61" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A61" s="0" t="s">
-        <v>198</v>
+        <v>201</v>
       </c>
       <c r="B61" s="0" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="C61" s="0" t="s">
-        <v>189</v>
+        <v>192</v>
       </c>
       <c r="D61" s="0" t="s">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="E61" s="0" t="s">
-        <v>199</v>
+        <v>202</v>
       </c>
       <c r="F61" s="0" t="s">
-        <v>200</v>
+        <v>203</v>
       </c>
       <c r="G61" s="0" t="s">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="H61" s="0" t="s">
-        <v>189</v>
+        <v>192</v>
       </c>
       <c r="I61" s="0" t="s">
-        <v>17</v>
+        <v>18</v>
+      </c>
+      <c r="J61" s="0" t="s">
+        <v>19</v>
       </c>
     </row>
     <row r="62" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A62" s="0" t="s">
-        <v>201</v>
+        <v>204</v>
       </c>
       <c r="B62" s="0" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="C62" s="0" t="s">
-        <v>189</v>
+        <v>192</v>
       </c>
       <c r="D62" s="0" t="s">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="E62" s="0" t="s">
-        <v>202</v>
+        <v>205</v>
       </c>
       <c r="F62" s="0" t="s">
-        <v>203</v>
+        <v>206</v>
       </c>
       <c r="G62" s="0" t="s">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="H62" s="0" t="s">
-        <v>189</v>
+        <v>192</v>
       </c>
       <c r="I62" s="0" t="s">
-        <v>17</v>
+        <v>18</v>
+      </c>
+      <c r="J62" s="0" t="s">
+        <v>19</v>
       </c>
     </row>
     <row r="63" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A63" s="0" t="s">
-        <v>204</v>
+        <v>207</v>
       </c>
       <c r="B63" s="0" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="C63" s="0" t="s">
-        <v>189</v>
+        <v>192</v>
       </c>
       <c r="D63" s="0" t="s">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="E63" s="0" t="s">
-        <v>205</v>
+        <v>208</v>
       </c>
       <c r="F63" s="0" t="s">
-        <v>206</v>
+        <v>209</v>
       </c>
       <c r="G63" s="0" t="s">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="H63" s="0" t="s">
-        <v>189</v>
+        <v>192</v>
       </c>
       <c r="I63" s="0" t="s">
-        <v>17</v>
+        <v>18</v>
+      </c>
+      <c r="J63" s="0" t="s">
+        <v>19</v>
       </c>
     </row>
     <row r="64" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A64" s="0" t="s">
-        <v>207</v>
+        <v>210</v>
       </c>
       <c r="B64" s="0" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="C64" s="0" t="s">
-        <v>189</v>
+        <v>192</v>
       </c>
       <c r="D64" s="0" t="s">
-        <v>34</v>
+        <v>36</v>
       </c>
       <c r="E64" s="0" t="s">
-        <v>208</v>
+        <v>211</v>
       </c>
       <c r="F64" s="0" t="s">
-        <v>209</v>
+        <v>212</v>
       </c>
       <c r="G64" s="0" t="s">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="H64" s="0" t="s">
-        <v>189</v>
+        <v>192</v>
       </c>
       <c r="I64" s="0" t="s">
-        <v>17</v>
+        <v>18</v>
+      </c>
+      <c r="J64" s="0" t="s">
+        <v>83</v>
       </c>
     </row>
     <row r="65" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A65" s="0" t="s">
-        <v>210</v>
+        <v>213</v>
       </c>
       <c r="B65" s="0" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="C65" s="0" t="s">
-        <v>189</v>
+        <v>192</v>
       </c>
       <c r="D65" s="0" t="s">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="E65" s="0" t="s">
-        <v>211</v>
+        <v>214</v>
       </c>
       <c r="F65" s="0" t="s">
-        <v>212</v>
+        <v>215</v>
       </c>
       <c r="G65" s="0" t="s">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="H65" s="0" t="s">
-        <v>189</v>
+        <v>192</v>
       </c>
       <c r="I65" s="0" t="s">
-        <v>17</v>
+        <v>18</v>
+      </c>
+      <c r="J65" s="0" t="s">
+        <v>19</v>
       </c>
     </row>
     <row r="66" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A66" s="0" t="s">
-        <v>213</v>
+        <v>216</v>
       </c>
       <c r="B66" s="0" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="C66" s="0" t="s">
-        <v>189</v>
+        <v>192</v>
       </c>
       <c r="D66" s="0" t="s">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="E66" s="0" t="s">
-        <v>214</v>
+        <v>217</v>
       </c>
       <c r="F66" s="0" t="s">
-        <v>215</v>
+        <v>218</v>
       </c>
       <c r="G66" s="0" t="s">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="H66" s="0" t="s">
-        <v>189</v>
+        <v>192</v>
       </c>
       <c r="I66" s="0" t="s">
-        <v>17</v>
+        <v>18</v>
+      </c>
+      <c r="J66" s="0" t="s">
+        <v>19</v>
       </c>
     </row>
     <row r="67" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A67" s="0" t="s">
-        <v>216</v>
+        <v>219</v>
       </c>
       <c r="B67" s="0" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="C67" s="0" t="s">
-        <v>189</v>
+        <v>192</v>
       </c>
       <c r="D67" s="0" t="s">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="E67" s="0" t="s">
-        <v>217</v>
+        <v>220</v>
       </c>
       <c r="F67" s="0" t="s">
-        <v>218</v>
+        <v>221</v>
       </c>
       <c r="G67" s="0" t="s">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="H67" s="0" t="s">
-        <v>189</v>
+        <v>192</v>
       </c>
       <c r="I67" s="0" t="s">
-        <v>17</v>
+        <v>18</v>
+      </c>
+      <c r="J67" s="0" t="s">
+        <v>19</v>
       </c>
     </row>
     <row r="68" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A68" s="0" t="s">
-        <v>219</v>
+        <v>222</v>
       </c>
       <c r="B68" s="0" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="C68" s="0" t="s">
-        <v>189</v>
+        <v>192</v>
       </c>
       <c r="D68" s="0" t="s">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="E68" s="0" t="s">
-        <v>220</v>
+        <v>223</v>
       </c>
       <c r="F68" s="0" t="s">
-        <v>221</v>
+        <v>224</v>
       </c>
       <c r="G68" s="0" t="s">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="H68" s="0" t="s">
-        <v>189</v>
+        <v>192</v>
       </c>
       <c r="I68" s="0" t="s">
-        <v>17</v>
+        <v>18</v>
+      </c>
+      <c r="J68" s="0" t="s">
+        <v>19</v>
       </c>
     </row>
     <row r="69" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A69" s="0" t="s">
-        <v>222</v>
+        <v>225</v>
       </c>
       <c r="B69" s="0" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="C69" s="0" t="s">
-        <v>189</v>
+        <v>192</v>
       </c>
       <c r="D69" s="0" t="s">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="E69" s="0" t="s">
-        <v>223</v>
+        <v>226</v>
       </c>
       <c r="F69" s="0" t="s">
-        <v>224</v>
+        <v>227</v>
       </c>
       <c r="G69" s="0" t="s">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="H69" s="0" t="s">
-        <v>189</v>
+        <v>192</v>
       </c>
       <c r="I69" s="0" t="s">
-        <v>17</v>
+        <v>18</v>
+      </c>
+      <c r="J69" s="0" t="s">
+        <v>19</v>
       </c>
     </row>
     <row r="70" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A70" s="0" t="s">
-        <v>225</v>
+        <v>228</v>
       </c>
       <c r="B70" s="0" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="C70" s="0" t="s">
-        <v>189</v>
+        <v>192</v>
       </c>
       <c r="D70" s="0" t="s">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="E70" s="0" t="s">
-        <v>226</v>
+        <v>229</v>
       </c>
       <c r="F70" s="0" t="s">
-        <v>227</v>
+        <v>230</v>
       </c>
       <c r="G70" s="0" t="s">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="H70" s="0" t="s">
-        <v>189</v>
+        <v>192</v>
       </c>
       <c r="I70" s="0" t="s">
-        <v>17</v>
+        <v>18</v>
+      </c>
+      <c r="J70" s="0" t="s">
+        <v>19</v>
       </c>
     </row>
     <row r="71" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A71" s="0" t="s">
-        <v>228</v>
+        <v>231</v>
       </c>
       <c r="B71" s="0" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="C71" s="0" t="s">
-        <v>189</v>
+        <v>192</v>
       </c>
       <c r="D71" s="0" t="s">
-        <v>34</v>
+        <v>36</v>
       </c>
       <c r="E71" s="0" t="s">
-        <v>229</v>
+        <v>232</v>
       </c>
       <c r="F71" s="0" t="s">
-        <v>230</v>
+        <v>233</v>
       </c>
       <c r="G71" s="0" t="s">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="H71" s="0" t="s">
-        <v>189</v>
+        <v>192</v>
       </c>
       <c r="I71" s="0" t="s">
-        <v>17</v>
+        <v>18</v>
+      </c>
+      <c r="J71" s="0" t="s">
+        <v>19</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
update compilation issues with dependency
</commit_message>
<xml_diff>
--- a/attendance/src/main/resources/LeaveDeductions.xlsx
+++ b/attendance/src/main/resources/LeaveDeductions.xlsx
@@ -835,8 +835,8 @@
   </sheetPr>
   <dimension ref="A1:J71"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A64" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A69" activeCellId="0" sqref="A69"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="G1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="J1" activeCellId="0" sqref="J1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15.75" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>

</xml_diff>

<commit_message>
Updated set data and missing changes
</commit_message>
<xml_diff>
--- a/attendance/src/main/resources/LeaveDeductions.xlsx
+++ b/attendance/src/main/resources/LeaveDeductions.xlsx
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="710" uniqueCount="234">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="851" uniqueCount="279">
   <si>
     <t xml:space="preserve">TCID</t>
   </si>
@@ -271,457 +271,592 @@
     <t xml:space="preserve">com.darwinbox.attendance.leavedeductions.totalduration.fullday.TestForTotalDurationFullDayDeduction</t>
   </si>
   <si>
+    <t xml:space="preserve">22</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Check Leave deductions when First Half leave is applied and approved for Total Work Duration Half day deduction</t>
+  </si>
+  <si>
+    <t xml:space="preserve">com.darwinbox.attendance.leavedeductions.totalduration.halfday.TestFirstHalfAppliedAndApprovedForTotalDurationHalfDayDeduction</t>
+  </si>
+  <si>
+    <t xml:space="preserve">23</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Check Leave deductions when First Half leave is applied and pending for Total Work Duration Half day deduction</t>
+  </si>
+  <si>
+    <t xml:space="preserve">com.darwinbox.attendance.leavedeductions.totalduration.halfday.TestFirstHalfAppliedAndPendingForTotalDurationHalfDayDeduction</t>
+  </si>
+  <si>
+    <t xml:space="preserve">24</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Check Leave deductions when Second Half leave is applied and approved for Total Work Duration Half day deduction</t>
+  </si>
+  <si>
+    <t xml:space="preserve">com.darwinbox.attendance.leavedeductions.totalduration.halfday.TestSecondHalfAppliedAndApprovedForTotalDurationHalfDayDeduction</t>
+  </si>
+  <si>
+    <t xml:space="preserve">25</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Check Leave deductions when Second Half leave is applied and pending for Total Work Duration Half day deduction</t>
+  </si>
+  <si>
+    <t xml:space="preserve">com.darwinbox.attendance.leavedeductions.totalduration.halfday.TestSecondHalfAppliedAndPendingForTotalDurationHalfDayDeduction</t>
+  </si>
+  <si>
+    <t xml:space="preserve">26</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Check Leave deductions when Full Day leave is applied and approved for Total Work Duration Half day deduction</t>
+  </si>
+  <si>
+    <t xml:space="preserve">com.darwinbox.attendance.leavedeductions.totalduration.halfday.TestFullDayAppliedAndApprovedForTotalDurationHalfDayDeduction</t>
+  </si>
+  <si>
+    <t xml:space="preserve">27</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Check Leave deductions when Full Day leave is applied and pending for Total Work Duration Half day deduction</t>
+  </si>
+  <si>
+    <t xml:space="preserve">com.darwinbox.attendance.leavedeductions.totalduration.halfday.TestFullDayAppliedAndPendingForTotalDurationHalfDayDeduction</t>
+  </si>
+  <si>
+    <t xml:space="preserve">28</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Check Leave deductions when no leave is applied for Total Work Duration Half day deduction</t>
+  </si>
+  <si>
+    <t xml:space="preserve">com.darwinbox.attendance.leavedeductions.totalduration.halfday.TestForTotalDurationHalfDayDeduction</t>
+  </si>
+  <si>
+    <t xml:space="preserve">29</t>
+  </si>
+  <si>
+    <t xml:space="preserve">FinalDuration</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Check Leave deductions when First Half leave is applied and approved for Final Work Duration Full day deduction</t>
+  </si>
+  <si>
+    <t xml:space="preserve">com.darwinbox.attendance.leavedeductions.finalduration.fullday.TestFirstHalfAppliedAndApprovedForFinalDurationFullDayDeduction</t>
+  </si>
+  <si>
+    <t xml:space="preserve">30</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Check Leave deductions when First Half leave is applied and pending for Final Work Duration Full day deduction</t>
+  </si>
+  <si>
+    <t xml:space="preserve">com.darwinbox.attendance.leavedeductions.finalduration.fullday.TestFirstHalfAppliedAndPendingForFinalDurationFullDayDeduction</t>
+  </si>
+  <si>
+    <t xml:space="preserve">31</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Check Leave deductions when Second Half leave is applied and approved for Final Work Duration Full day deduction</t>
+  </si>
+  <si>
+    <t xml:space="preserve">com.darwinbox.attendance.leavedeductions.finalduration.fullday.TestSecondHalfAppliedAndApprovedForFinalDurationFullDayDeduction</t>
+  </si>
+  <si>
+    <t xml:space="preserve">32</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Check Leave deductions when Second Half leave is applied and pending for Final Work Duration Full day deduction</t>
+  </si>
+  <si>
+    <t xml:space="preserve">com.darwinbox.attendance.leavedeductions.finalduration.fullday.TestSecondHalfAppliedAndPendingForFinalDurationFullDayDeduction</t>
+  </si>
+  <si>
+    <t xml:space="preserve">33</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Check Leave deductions when Full Day leave is applied and approved for Final Work Duration Full day deduction</t>
+  </si>
+  <si>
+    <t xml:space="preserve">com.darwinbox.attendance.leavedeductions.finalduration.fullday.TestFullDayAppliedAndApprovedForFinalDurationFullDayDeduction</t>
+  </si>
+  <si>
+    <t xml:space="preserve">34</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Check Leave deductions when Full Day leave is applied and pending for Final Work Duration Full day deduction</t>
+  </si>
+  <si>
+    <t xml:space="preserve">com.darwinbox.attendance.leavedeductions.finalduration.fullday.TestFullDayAppliedAndPendingForFinalDurationFullDayDeduction</t>
+  </si>
+  <si>
+    <t xml:space="preserve">35</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Check Leave deductions when no leave is applied for Final Work Duration Full day deduction</t>
+  </si>
+  <si>
+    <t xml:space="preserve">com.darwinbox.attendance.leavedeductions.finalduration.fullday.TestForFinalDurationFullDayDeduction</t>
+  </si>
+  <si>
+    <t xml:space="preserve">36</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Check Leave deductions when First Half leave is applied and approved for Final Work Duration Half day deduction</t>
+  </si>
+  <si>
+    <t xml:space="preserve">com.darwinbox.attendance.leavedeductions.finalduration.halfday.TestFirstHalfAppliedAndApprovedForFinalDurationHalfDayDeduction</t>
+  </si>
+  <si>
+    <t xml:space="preserve">37</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Check Leave deductions when First Half leave is applied and pending for Final Work Duration Half day deduction</t>
+  </si>
+  <si>
+    <t xml:space="preserve">com.darwinbox.attendance.leavedeductions.finalduration.halfday.TestFirstHalfAppliedAndPendingForFinalDurationHalfDayDeduction</t>
+  </si>
+  <si>
+    <t xml:space="preserve">38</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Check Leave deductions when Second Half leave is applied and approved for Final Work Duration Half day deduction</t>
+  </si>
+  <si>
+    <t xml:space="preserve">com.darwinbox.attendance.leavedeductions.finalduration.halfday.TestSecondHalfAppliedAndApprovedForFinalDurationHalfDayDeduction</t>
+  </si>
+  <si>
+    <t xml:space="preserve">39</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Check Leave deductions when Second Half leave is applied and pending for Final Work Duration Half day deduction</t>
+  </si>
+  <si>
+    <t xml:space="preserve">com.darwinbox.attendance.leavedeductions.finalduration.halfday.TestSecondHalfAppliedAndPendingForFinalDurationHalfDayDeduction</t>
+  </si>
+  <si>
+    <t xml:space="preserve">40</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Check Leave deductions when Full Day leave is applied and approved for Final Work Duration Half day deduction</t>
+  </si>
+  <si>
+    <t xml:space="preserve">com.darwinbox.attendance.leavedeductions.finalduration.halfday.TestFullDayAppliedAndApprovedForFinalDurationHalfDayDeduction</t>
+  </si>
+  <si>
+    <t xml:space="preserve">41</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Check Leave deductions when Full Day leave is applied and pending for Final Work Duration Half day deduction</t>
+  </si>
+  <si>
+    <t xml:space="preserve">com.darwinbox.attendance.leavedeductions.finalduration.halfday.TestFullDayAppliedAndPendingForFinalDurationHalfDayDeduction</t>
+  </si>
+  <si>
+    <t xml:space="preserve">42</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Check Leave deductions when no leave is applied for Final Work Duration Half day deduction</t>
+  </si>
+  <si>
+    <t xml:space="preserve">com.darwinbox.attendance.leavedeductions.finalduration.halfday.TestForFinalDurationHalfDayDeduction</t>
+  </si>
+  <si>
+    <t xml:space="preserve">43</t>
+  </si>
+  <si>
+    <t xml:space="preserve">LateDuration</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Check Leave deductions when First Half leave is applied and approved for Late Duration Full day deduction</t>
+  </si>
+  <si>
+    <t xml:space="preserve">com.darwinbox.attendance.leavedeductions.lateduration.fullday.TestFirstHalfAppliedAndApprovedForLateByFullDayDeduction</t>
+  </si>
+  <si>
+    <t xml:space="preserve">44</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Check Leave deductions when First Half leave is applied and pending for Late Duration Full day deduction</t>
+  </si>
+  <si>
+    <t xml:space="preserve">com.darwinbox.attendance.leavedeductions.lateduration.fullday.TestFirstHalfAppliedAndPendingForLateByFullDayDeduction</t>
+  </si>
+  <si>
+    <t xml:space="preserve">45</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Check Leave deductions when Second Half leave is applied and approved for Late Duration Full day deduction</t>
+  </si>
+  <si>
+    <t xml:space="preserve">com.darwinbox.attendance.leavedeductions.lateduration.fullday.TestSecondHalfAppliedAndApprovedForLateByFullDayDeduction</t>
+  </si>
+  <si>
+    <t xml:space="preserve">46</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Check Leave deductions when Second Half leave is applied and pending for Late Duration Full day deduction</t>
+  </si>
+  <si>
+    <t xml:space="preserve">com.darwinbox.attendance.leavedeductions.lateduration.fullday.TestSecondHalfAppliedAndPendingForLateByFullDayDeduction</t>
+  </si>
+  <si>
+    <t xml:space="preserve">47</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Check Leave deductions when Full Day leave is applied and approved for Late Duration Full day deduction</t>
+  </si>
+  <si>
+    <t xml:space="preserve">com.darwinbox.attendance.leavedeductions.lateduration.fullday.TestFullDayAppliedAndApprovedForLateByFullDayDeduction</t>
+  </si>
+  <si>
+    <t xml:space="preserve">48</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Check Leave deductions when Full Day leave is applied and pending for Late Duration Full day deduction</t>
+  </si>
+  <si>
+    <t xml:space="preserve">com.darwinbox.attendance.leavedeductions.lateduration.fullday.TestFullDayAppliedAndPendingForLateByFullDayDeduction</t>
+  </si>
+  <si>
+    <t xml:space="preserve">49</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Check Leave deductions when no leave is applied for Late Duration Full day deduction</t>
+  </si>
+  <si>
+    <t xml:space="preserve">com.darwinbox.attendance.leavedeductions.lateduration.fullday.TestForLateByFullDayDeduction</t>
+  </si>
+  <si>
+    <t xml:space="preserve">50</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Check Leave deductions when First Half leave is applied and approved for Late Duration Half day deduction</t>
+  </si>
+  <si>
+    <t xml:space="preserve">com.darwinbox.attendance.leavedeductions.lateduration.halfday.TestFirstHalfAppliedAndApprovedForLateByHalfDayDeduction</t>
+  </si>
+  <si>
+    <t xml:space="preserve">51</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Check Leave deductions when First Half leave is applied and pending for Late Duration Half day deduction</t>
+  </si>
+  <si>
+    <t xml:space="preserve">com.darwinbox.attendance.leavedeductions.lateduration.halfday.TestFirstHalfAppliedAndPendingForLateByHalfDayDeduction</t>
+  </si>
+  <si>
+    <t xml:space="preserve">52</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Check Leave deductions when Second Half leave is applied and approved for Late Duration Half day deduction</t>
+  </si>
+  <si>
+    <t xml:space="preserve">com.darwinbox.attendance.leavedeductions.lateduration.halfday.TestSecondHalfAppliedAndApprovedForLateByHalfDayDeduction</t>
+  </si>
+  <si>
+    <t xml:space="preserve">53</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Check Leave deductions when Second Half leave is applied and pending for Late Duration Half day deduction</t>
+  </si>
+  <si>
+    <t xml:space="preserve">com.darwinbox.attendance.leavedeductions.lateduration.halfday.TestSecondHalfAppliedAndPendingForLateByHalfDayDeduction</t>
+  </si>
+  <si>
+    <t xml:space="preserve">54</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Check Leave deductions when Full Day leave is applied and approved for Late Duration Half day deduction</t>
+  </si>
+  <si>
+    <t xml:space="preserve">com.darwinbox.attendance.leavedeductions.lateduration.halfday.TestFullDayAppliedAndApprovedForLateByHalfDayDeduction</t>
+  </si>
+  <si>
+    <t xml:space="preserve">55</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Check Leave deductions when Full Day leave is applied and pending for Late Duration Half day deduction</t>
+  </si>
+  <si>
+    <t xml:space="preserve">com.darwinbox.attendance.leavedeductions.lateduration.halfday.TestFullDayAppliedAndPendingForLateByHalfDayDeduction</t>
+  </si>
+  <si>
+    <t xml:space="preserve">56</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Check Leave deductions when no leave is applied for Late Duration Half day deduction</t>
+  </si>
+  <si>
+    <t xml:space="preserve">com.darwinbox.attendance.leavedeductions.lateduration.halfday.TestForLateByHalfDayDeduction</t>
+  </si>
+  <si>
+    <t xml:space="preserve">57</t>
+  </si>
+  <si>
+    <t xml:space="preserve">EarlyDuration</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Check Leave deductions when First Half leave is applied and approved for Early Duration Full day deduction</t>
+  </si>
+  <si>
+    <t xml:space="preserve">com.darwinbox.attendance.leavedeductions.earlyduration.fullday.TestFirstHalfAppliedAndApprovedForEarlyByFullDayDeduction</t>
+  </si>
+  <si>
+    <t xml:space="preserve">58</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Check Leave deductions when First Half leave is applied and pending for Early Duration Full day deduction</t>
+  </si>
+  <si>
+    <t xml:space="preserve">com.darwinbox.attendance.leavedeductions.earlyduration.fullday.TestFirstHalfAppliedAndPendingForEarlyByFullDayDeduction</t>
+  </si>
+  <si>
+    <t xml:space="preserve">59</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Check Leave deductions when Second Half leave is applied and approved for Early Duration Full day deduction</t>
+  </si>
+  <si>
+    <t xml:space="preserve">com.darwinbox.attendance.leavedeductions.earlyduration.fullday.TestSecondHalfAppliedAndApprovedForEarlyByFullDayDeduction</t>
+  </si>
+  <si>
+    <t xml:space="preserve">60</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Check Leave deductions when Second Half leave is applied and pending for Early Duration Full day deduction</t>
+  </si>
+  <si>
+    <t xml:space="preserve">com.darwinbox.attendance.leavedeductions.earlyduration.fullday.TestSecondHalfAppliedAndPendingForEarlyByFullDayDeduction</t>
+  </si>
+  <si>
+    <t xml:space="preserve">61</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Check Leave deductions when Full Day leave is applied and approved for Early Duration Full day deduction</t>
+  </si>
+  <si>
+    <t xml:space="preserve">com.darwinbox.attendance.leavedeductions.earlyduration.fullday.TestFullDayAppliedAndApprovedForEarlyByFullDayDeduction</t>
+  </si>
+  <si>
+    <t xml:space="preserve">62</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Check Leave deductions when Full Day leave is applied and pending for Early Duration Full day deduction</t>
+  </si>
+  <si>
+    <t xml:space="preserve">com.darwinbox.attendance.leavedeductions.earlyduration.fullday.TestFullDayAppliedAndPendingForEarlyByFullDayDeduction</t>
+  </si>
+  <si>
+    <t xml:space="preserve">63</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Check Leave deductions when no leave is applied for Early Duration Full day deduction</t>
+  </si>
+  <si>
+    <t xml:space="preserve">com.darwinbox.attendance.leavedeductions.earlyduration.fullday.TestForEarlyByFullDayDeduction</t>
+  </si>
+  <si>
+    <t xml:space="preserve">64</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Check Leave deductions when First Half leave is applied and approved for Early Duration Half day deduction</t>
+  </si>
+  <si>
+    <t xml:space="preserve">com.darwinbox.attendance.leavedeductions.earlyduration.halfday.TestFirstHalfAppliedAndApprovedForEarlyByHalfDayDeduction</t>
+  </si>
+  <si>
+    <t xml:space="preserve">65</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Check Leave deductions when First Half leave is applied and pending for Early Duration Half day deduction</t>
+  </si>
+  <si>
+    <t xml:space="preserve">com.darwinbox.attendance.leavedeductions.earlyduration.halfday.TestFirstHalfAppliedAndPendingForEarlyByHalfDayDeduction</t>
+  </si>
+  <si>
+    <t xml:space="preserve">66</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Check Leave deductions when Second Half leave is applied and approved for Early Duration Half day deduction</t>
+  </si>
+  <si>
+    <t xml:space="preserve">com.darwinbox.attendance.leavedeductions.earlyduration.halfday.TestSecondHalfAppliedAndApprovedForEarlyByHalfDayDeduction</t>
+  </si>
+  <si>
+    <t xml:space="preserve">67</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Check Leave deductions when Second Half leave is applied and pending for Early Duration Half day deduction</t>
+  </si>
+  <si>
+    <t xml:space="preserve">com.darwinbox.attendance.leavedeductions.earlyduration.halfday.TestSecondHalfAppliedAndPendingForEarlyByHalfDayDeduction</t>
+  </si>
+  <si>
+    <t xml:space="preserve">68</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Check Leave deductions when Full Day leave is applied and approved for Early Duration Half day deduction</t>
+  </si>
+  <si>
+    <t xml:space="preserve">com.darwinbox.attendance.leavedeductions.earlyduration.halfday.TestFullDayAppliedAndApprovedForEarlyByHalfDayDeduction</t>
+  </si>
+  <si>
+    <t xml:space="preserve">69</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Check Leave deductions when Full Day leave is applied and pending for Early Duration Half day deduction</t>
+  </si>
+  <si>
+    <t xml:space="preserve">com.darwinbox.attendance.leavedeductions.earlyduration.halfday.TestFullDayAppliedAndPendingForEarlyByHalfDayDeduction</t>
+  </si>
+  <si>
+    <t xml:space="preserve">70</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Check Leave deductions when no leave is applied for Early Duration Half day deduction</t>
+  </si>
+  <si>
+    <t xml:space="preserve">com.darwinbox.attendance.leavedeductions.earlyduration.halfday.TestForEarlyByHalfDayDeduction</t>
+  </si>
+  <si>
+    <t xml:space="preserve">71</t>
+  </si>
+  <si>
+    <t xml:space="preserve">LateMark</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Check Leave deductions when First Half leave is applied and approved for Late Mark Full day deduction</t>
+  </si>
+  <si>
+    <t xml:space="preserve">com.darwinbox.attendance.leavedeductions.latemark.fullday.TestFirstHalfAppliedAndApprovedForLateMarkFullDayDeduction</t>
+  </si>
+  <si>
+    <t xml:space="preserve">LateMarkFullDay</t>
+  </si>
+  <si>
     <t xml:space="preserve">yes</t>
   </si>
   <si>
-    <t xml:space="preserve">22</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Check Leave deductions when First Half leave is applied and approved for Total Work Duration Half day deduction</t>
-  </si>
-  <si>
-    <t xml:space="preserve">com.darwinbox.attendance.leavedeductions.totalduration.halfday.TestFirstHalfAppliedAndApprovedForTotalDurationHalfDayDeduction</t>
-  </si>
-  <si>
-    <t xml:space="preserve">23</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Check Leave deductions when First Half leave is applied and pending for Total Work Duration Half day deduction</t>
-  </si>
-  <si>
-    <t xml:space="preserve">com.darwinbox.attendance.leavedeductions.totalduration.halfday.TestFirstHalfAppliedAndPendingForTotalDurationHalfDayDeduction</t>
-  </si>
-  <si>
-    <t xml:space="preserve">24</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Check Leave deductions when Second Half leave is applied and approved for Total Work Duration Half day deduction</t>
-  </si>
-  <si>
-    <t xml:space="preserve">com.darwinbox.attendance.leavedeductions.totalduration.halfday.TestSecondHalfAppliedAndApprovedForTotalDurationHalfDayDeduction</t>
-  </si>
-  <si>
-    <t xml:space="preserve">25</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Check Leave deductions when Second Half leave is applied and pending for Total Work Duration Half day deduction</t>
-  </si>
-  <si>
-    <t xml:space="preserve">com.darwinbox.attendance.leavedeductions.totalduration.halfday.TestSecondHalfAppliedAndPendingForTotalDurationHalfDayDeduction</t>
-  </si>
-  <si>
-    <t xml:space="preserve">26</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Check Leave deductions when Full Day leave is applied and approved for Total Work Duration Half day deduction</t>
-  </si>
-  <si>
-    <t xml:space="preserve">com.darwinbox.attendance.leavedeductions.totalduration.halfday.TestFullDayAppliedAndApprovedForTotalDurationHalfDayDeduction</t>
-  </si>
-  <si>
-    <t xml:space="preserve">27</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Check Leave deductions when Full Day leave is applied and pending for Total Work Duration Half day deduction</t>
-  </si>
-  <si>
-    <t xml:space="preserve">com.darwinbox.attendance.leavedeductions.totalduration.halfday.TestFullDayAppliedAndPendingForTotalDurationHalfDayDeduction</t>
-  </si>
-  <si>
-    <t xml:space="preserve">28</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Check Leave deductions when no leave is applied for Total Work Duration Half day deduction</t>
-  </si>
-  <si>
-    <t xml:space="preserve">com.darwinbox.attendance.leavedeductions.totalduration.halfday.TestForTotalDurationHalfDayDeduction</t>
-  </si>
-  <si>
-    <t xml:space="preserve">29</t>
-  </si>
-  <si>
-    <t xml:space="preserve">FinalDuration</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Check Leave deductions when First Half leave is applied and approved for Final Work Duration Full day deduction</t>
-  </si>
-  <si>
-    <t xml:space="preserve">com.darwinbox.attendance.leavedeductions.finalduration.fullday.TestFirstHalfAppliedAndApprovedForFinalDurationFullDayDeduction</t>
-  </si>
-  <si>
-    <t xml:space="preserve">30</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Check Leave deductions when First Half leave is applied and pending for Final Work Duration Full day deduction</t>
-  </si>
-  <si>
-    <t xml:space="preserve">com.darwinbox.attendance.leavedeductions.finalduration.fullday.TestFirstHalfAppliedAndPendingForFinalDurationFullDayDeduction</t>
-  </si>
-  <si>
-    <t xml:space="preserve">31</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Check Leave deductions when Second Half leave is applied and approved for Final Work Duration Full day deduction</t>
-  </si>
-  <si>
-    <t xml:space="preserve">com.darwinbox.attendance.leavedeductions.finalduration.fullday.TestSecondHalfAppliedAndApprovedForFinalDurationFullDayDeduction</t>
-  </si>
-  <si>
-    <t xml:space="preserve">32</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Check Leave deductions when Second Half leave is applied and pending for Final Work Duration Full day deduction</t>
-  </si>
-  <si>
-    <t xml:space="preserve">com.darwinbox.attendance.leavedeductions.finalduration.fullday.TestSecondHalfAppliedAndPendingForFinalDurationFullDayDeduction</t>
-  </si>
-  <si>
-    <t xml:space="preserve">33</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Check Leave deductions when Full Day leave is applied and approved for Final Work Duration Full day deduction</t>
-  </si>
-  <si>
-    <t xml:space="preserve">com.darwinbox.attendance.leavedeductions.finalduration.fullday.TestFullDayAppliedAndApprovedForFinalDurationFullDayDeduction</t>
-  </si>
-  <si>
-    <t xml:space="preserve">34</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Check Leave deductions when Full Day leave is applied and pending for Final Work Duration Full day deduction</t>
-  </si>
-  <si>
-    <t xml:space="preserve">com.darwinbox.attendance.leavedeductions.finalduration.fullday.TestFullDayAppliedAndPendingForFinalDurationFullDayDeduction</t>
-  </si>
-  <si>
-    <t xml:space="preserve">35</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Check Leave deductions when no leave is applied for Final Work Duration Full day deduction</t>
-  </si>
-  <si>
-    <t xml:space="preserve">com.darwinbox.attendance.leavedeductions.finalduration.fullday.TestForFinalDurationFullDayDeduction</t>
-  </si>
-  <si>
-    <t xml:space="preserve">36</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Check Leave deductions when First Half leave is applied and approved for Final Work Duration Half day deduction</t>
-  </si>
-  <si>
-    <t xml:space="preserve">com.darwinbox.attendance.leavedeductions.finalduration.halfday.TestFirstHalfAppliedAndApprovedForFinalDurationHalfDayDeduction</t>
-  </si>
-  <si>
-    <t xml:space="preserve">37</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Check Leave deductions when First Half leave is applied and pending for Final Work Duration Half day deduction</t>
-  </si>
-  <si>
-    <t xml:space="preserve">com.darwinbox.attendance.leavedeductions.finalduration.halfday.TestFirstHalfAppliedAndPendingForFinalDurationHalfDayDeduction</t>
-  </si>
-  <si>
-    <t xml:space="preserve">38</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Check Leave deductions when Second Half leave is applied and approved for Final Work Duration Half day deduction</t>
-  </si>
-  <si>
-    <t xml:space="preserve">com.darwinbox.attendance.leavedeductions.finalduration.halfday.TestSecondHalfAppliedAndApprovedForFinalDurationHalfDayDeduction</t>
-  </si>
-  <si>
-    <t xml:space="preserve">39</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Check Leave deductions when Second Half leave is applied and pending for Final Work Duration Half day deduction</t>
-  </si>
-  <si>
-    <t xml:space="preserve">com.darwinbox.attendance.leavedeductions.finalduration.halfday.TestSecondHalfAppliedAndPendingForFinalDurationHalfDayDeduction</t>
-  </si>
-  <si>
-    <t xml:space="preserve">40</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Check Leave deductions when Full Day leave is applied and approved for Final Work Duration Half day deduction</t>
-  </si>
-  <si>
-    <t xml:space="preserve">com.darwinbox.attendance.leavedeductions.finalduration.halfday.TestFullDayAppliedAndApprovedForFinalDurationHalfDayDeduction</t>
-  </si>
-  <si>
-    <t xml:space="preserve">41</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Check Leave deductions when Full Day leave is applied and pending for Final Work Duration Half day deduction</t>
-  </si>
-  <si>
-    <t xml:space="preserve">com.darwinbox.attendance.leavedeductions.finalduration.halfday.TestFullDayAppliedAndPendingForFinalDurationHalfDayDeduction</t>
-  </si>
-  <si>
-    <t xml:space="preserve">42</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Check Leave deductions when no leave is applied for Final Work Duration Half day deduction</t>
-  </si>
-  <si>
-    <t xml:space="preserve">com.darwinbox.attendance.leavedeductions.finalduration.halfday.TestForFinalDurationHalfDayDeduction</t>
-  </si>
-  <si>
-    <t xml:space="preserve">43</t>
-  </si>
-  <si>
-    <t xml:space="preserve">LateDuration</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Check Leave deductions when First Half leave is applied and approved for Late Duration Full day deduction</t>
-  </si>
-  <si>
-    <t xml:space="preserve">com.darwinbox.attendance.leavedeductions.lateduration.fullday.TestFirstHalfAppliedAndApprovedForLateByFullDayDeduction</t>
-  </si>
-  <si>
-    <t xml:space="preserve">44</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Check Leave deductions when First Half leave is applied and pending for Late Duration Full day deduction</t>
-  </si>
-  <si>
-    <t xml:space="preserve">com.darwinbox.attendance.leavedeductions.lateduration.fullday.TestFirstHalfAppliedAndPendingForLateByFullDayDeduction</t>
-  </si>
-  <si>
-    <t xml:space="preserve">45</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Check Leave deductions when Second Half leave is applied and approved for Late Duration Full day deduction</t>
-  </si>
-  <si>
-    <t xml:space="preserve">com.darwinbox.attendance.leavedeductions.lateduration.fullday.TestSecondHalfAppliedAndApprovedForLateByFullDayDeduction</t>
-  </si>
-  <si>
-    <t xml:space="preserve">46</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Check Leave deductions when Second Half leave is applied and pending for Late Duration Full day deduction</t>
-  </si>
-  <si>
-    <t xml:space="preserve">com.darwinbox.attendance.leavedeductions.lateduration.fullday.TestSecondHalfAppliedAndPendingForLateByFullDayDeduction</t>
-  </si>
-  <si>
-    <t xml:space="preserve">47</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Check Leave deductions when Full Day leave is applied and approved for Late Duration Full day deduction</t>
-  </si>
-  <si>
-    <t xml:space="preserve">com.darwinbox.attendance.leavedeductions.lateduration.fullday.TestFullDayAppliedAndApprovedForLateByFullDayDeduction</t>
-  </si>
-  <si>
-    <t xml:space="preserve">48</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Check Leave deductions when Full Day leave is applied and pending for Late Duration Full day deduction</t>
-  </si>
-  <si>
-    <t xml:space="preserve">com.darwinbox.attendance.leavedeductions.lateduration.fullday.TestFullDayAppliedAndPendingForLateByFullDayDeduction</t>
-  </si>
-  <si>
-    <t xml:space="preserve">49</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Check Leave deductions when no leave is applied for Late Duration Full day deduction</t>
-  </si>
-  <si>
-    <t xml:space="preserve">com.darwinbox.attendance.leavedeductions.lateduration.fullday.TestForLateByFullDayDeduction</t>
-  </si>
-  <si>
-    <t xml:space="preserve">50</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Check Leave deductions when First Half leave is applied and approved for Late Duration Half day deduction</t>
-  </si>
-  <si>
-    <t xml:space="preserve">com.darwinbox.attendance.leavedeductions.lateduration.halfday.TestFirstHalfAppliedAndApprovedForLateByHalfDayDeduction</t>
-  </si>
-  <si>
-    <t xml:space="preserve">51</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Check Leave deductions when First Half leave is applied and pending for Late Duration Half day deduction</t>
-  </si>
-  <si>
-    <t xml:space="preserve">com.darwinbox.attendance.leavedeductions.lateduration.halfday.TestFirstHalfAppliedAndPendingForLateByHalfDayDeduction</t>
-  </si>
-  <si>
-    <t xml:space="preserve">52</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Check Leave deductions when Second Half leave is applied and approved for Late Duration Half day deduction</t>
-  </si>
-  <si>
-    <t xml:space="preserve">com.darwinbox.attendance.leavedeductions.lateduration.halfday.TestSecondHalfAppliedAndApprovedForLateByHalfDayDeduction</t>
-  </si>
-  <si>
-    <t xml:space="preserve">53</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Check Leave deductions when Second Half leave is applied and pending for Late Duration Half day deduction</t>
-  </si>
-  <si>
-    <t xml:space="preserve">com.darwinbox.attendance.leavedeductions.lateduration.halfday.TestSecondHalfAppliedAndPendingForLateByHalfDayDeduction</t>
-  </si>
-  <si>
-    <t xml:space="preserve">54</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Check Leave deductions when Full Day leave is applied and approved for Late Duration Half day deduction</t>
-  </si>
-  <si>
-    <t xml:space="preserve">com.darwinbox.attendance.leavedeductions.lateduration.halfday.TestFullDayAppliedAndApprovedForLateByHalfDayDeduction</t>
-  </si>
-  <si>
-    <t xml:space="preserve">55</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Check Leave deductions when Full Day leave is applied and pending for Late Duration Half day deduction</t>
-  </si>
-  <si>
-    <t xml:space="preserve">com.darwinbox.attendance.leavedeductions.lateduration.halfday.TestFullDayAppliedAndPendingForLateByHalfDayDeduction</t>
-  </si>
-  <si>
-    <t xml:space="preserve">56</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Check Leave deductions when no leave is applied for Late Duration Half day deduction</t>
-  </si>
-  <si>
-    <t xml:space="preserve">com.darwinbox.attendance.leavedeductions.lateduration.halfday.TestForLateByHalfDayDeduction</t>
-  </si>
-  <si>
-    <t xml:space="preserve">57</t>
-  </si>
-  <si>
-    <t xml:space="preserve">EarlyDuration</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Check Leave deductions when First Half leave is applied and approved for Early Duration Full day deduction</t>
-  </si>
-  <si>
-    <t xml:space="preserve">com.darwinbox.attendance.leavedeductions.earlyduration.fullday.TestFirstHalfAppliedAndApprovedForEarlyByFullDayDeduction</t>
-  </si>
-  <si>
-    <t xml:space="preserve">58</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Check Leave deductions when First Half leave is applied and pending for Early Duration Full day deduction</t>
-  </si>
-  <si>
-    <t xml:space="preserve">com.darwinbox.attendance.leavedeductions.earlyduration.fullday.TestFirstHalfAppliedAndPendingForEarlyByFullDayDeduction</t>
-  </si>
-  <si>
-    <t xml:space="preserve">59</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Check Leave deductions when Second Half leave is applied and approved for Early Duration Full day deduction</t>
-  </si>
-  <si>
-    <t xml:space="preserve">com.darwinbox.attendance.leavedeductions.earlyduration.fullday.TestSecondHalfAppliedAndApprovedForEarlyByFullDayDeduction</t>
-  </si>
-  <si>
-    <t xml:space="preserve">60</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Check Leave deductions when Second Half leave is applied and pending for Early Duration Full day deduction</t>
-  </si>
-  <si>
-    <t xml:space="preserve">com.darwinbox.attendance.leavedeductions.earlyduration.fullday.TestSecondHalfAppliedAndPendingForEarlyByFullDayDeduction</t>
-  </si>
-  <si>
-    <t xml:space="preserve">61</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Check Leave deductions when Full Day leave is applied and approved for Early Duration Full day deduction</t>
-  </si>
-  <si>
-    <t xml:space="preserve">com.darwinbox.attendance.leavedeductions.earlyduration.fullday.TestFullDayAppliedAndApprovedForEarlyByFullDayDeduction</t>
-  </si>
-  <si>
-    <t xml:space="preserve">62</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Check Leave deductions when Full Day leave is applied and pending for Early Duration Full day deduction</t>
-  </si>
-  <si>
-    <t xml:space="preserve">com.darwinbox.attendance.leavedeductions.earlyduration.fullday.TestFullDayAppliedAndPendingForEarlyByFullDayDeduction</t>
-  </si>
-  <si>
-    <t xml:space="preserve">63</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Check Leave deductions when no leave is applied for Early Duration Full day deduction</t>
-  </si>
-  <si>
-    <t xml:space="preserve">com.darwinbox.attendance.leavedeductions.earlyduration.fullday.TestForEarlyByFullDayDeduction</t>
-  </si>
-  <si>
-    <t xml:space="preserve">64</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Check Leave deductions when First Half leave is applied and approved for Early Duration Half day deduction</t>
-  </si>
-  <si>
-    <t xml:space="preserve">com.darwinbox.attendance.leavedeductions.earlyduration.halfday.TestFirstHalfAppliedAndApprovedForEarlyByHalfDayDeduction</t>
-  </si>
-  <si>
-    <t xml:space="preserve">65</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Check Leave deductions when First Half leave is applied and pending for Early Duration Half day deduction</t>
-  </si>
-  <si>
-    <t xml:space="preserve">com.darwinbox.attendance.leavedeductions.earlyduration.halfday.TestFirstHalfAppliedAndPendingForEarlyByHalfDayDeduction</t>
-  </si>
-  <si>
-    <t xml:space="preserve">66</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Check Leave deductions when Second Half leave is applied and approved for Early Duration Half day deduction</t>
-  </si>
-  <si>
-    <t xml:space="preserve">com.darwinbox.attendance.leavedeductions.earlyduration.halfday.TestSecondHalfAppliedAndApprovedForEarlyByHalfDayDeduction</t>
-  </si>
-  <si>
-    <t xml:space="preserve">67</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Check Leave deductions when Second Half leave is applied and pending for Early Duration Half day deduction</t>
-  </si>
-  <si>
-    <t xml:space="preserve">com.darwinbox.attendance.leavedeductions.earlyduration.halfday.TestSecondHalfAppliedAndPendingForEarlyByHalfDayDeduction</t>
-  </si>
-  <si>
-    <t xml:space="preserve">68</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Check Leave deductions when Full Day leave is applied and approved for Early Duration Half day deduction</t>
-  </si>
-  <si>
-    <t xml:space="preserve">com.darwinbox.attendance.leavedeductions.earlyduration.halfday.TestFullDayAppliedAndApprovedForEarlyByHalfDayDeduction</t>
-  </si>
-  <si>
-    <t xml:space="preserve">69</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Check Leave deductions when Full Day leave is applied and pending for Early Duration Half day deduction</t>
-  </si>
-  <si>
-    <t xml:space="preserve">com.darwinbox.attendance.leavedeductions.earlyduration.halfday.TestFullDayAppliedAndPendingForEarlyByHalfDayDeduction</t>
-  </si>
-  <si>
-    <t xml:space="preserve">70</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Check Leave deductions when no leave is applied for Early Duration Half day deduction</t>
-  </si>
-  <si>
-    <t xml:space="preserve">com.darwinbox.attendance.leavedeductions.earlyduration.halfday.TestForEarlyByHalfDayDeduction</t>
+    <t xml:space="preserve">72</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Check Leave deductions when First Half leave is applied and pending for Late Mark Full day deduction</t>
+  </si>
+  <si>
+    <t xml:space="preserve">com.darwinbox.attendance.leavedeductions.latemark.fullday.TestFirstHalfAppliedAndPendingForLateMarkFullDayDeduction</t>
+  </si>
+  <si>
+    <t xml:space="preserve">73</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Check Leave deductions when Second Half leave is applied and approved for Late Mark Full day deduction</t>
+  </si>
+  <si>
+    <t xml:space="preserve">com.darwinbox.attendance.leavedeductions.latemark.fullday.TestSecondHalfAppliedAndApprovedForLateMarkFullDayDeduction</t>
+  </si>
+  <si>
+    <t xml:space="preserve">74</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Check Leave deductions when Second Half leave is applied and pending for Late Mark Full day deduction</t>
+  </si>
+  <si>
+    <t xml:space="preserve">com.darwinbox.attendance.leavedeductions.latemark.fullday.TestSecondHalfAppliedAndPendingForLateMarkFullDayDeduction</t>
+  </si>
+  <si>
+    <t xml:space="preserve">75</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Check Leave deductions when Full Day leave is applied and approved for Late Mark Full day deduction</t>
+  </si>
+  <si>
+    <t xml:space="preserve">com.darwinbox.attendance.leavedeductions.latemark.fullday.TestFullDayAppliedAndApprovedForLateMarkFullDayDeduction</t>
+  </si>
+  <si>
+    <t xml:space="preserve">76</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Check Leave deductions when Full Day leave is applied and pending for Late Mark Full day deduction</t>
+  </si>
+  <si>
+    <t xml:space="preserve">com.darwinbox.attendance.leavedeductions.latemark.fullday.TestFullDayAppliedAndPendingForLateMarkFullDayDeduction</t>
+  </si>
+  <si>
+    <t xml:space="preserve">77</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Check Leave deductions when no leave is applied for Late Mark Full day deduction</t>
+  </si>
+  <si>
+    <t xml:space="preserve">com.darwinbox.attendance.leavedeductions.latemark.fullday.TestForLateMarkFullDayDeduction</t>
+  </si>
+  <si>
+    <t xml:space="preserve">78</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Check Leave deductions when First Half leave is applied and approved for Late Mark Half day deduction</t>
+  </si>
+  <si>
+    <t xml:space="preserve">com.darwinbox.attendance.leavedeductions.latemark.halfday.TestFirstHalfAppliedAndApprovedForLateMarkHalfDayDeduction</t>
+  </si>
+  <si>
+    <t xml:space="preserve">LateMarkHalfDay</t>
+  </si>
+  <si>
+    <t xml:space="preserve">79</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Check Leave deductions when First Half leave is applied and pending for Late Mark Half day deduction</t>
+  </si>
+  <si>
+    <t xml:space="preserve">com.darwinbox.attendance.leavedeductions.latemark.halfday.TestFirstHalfAppliedAndPendingForLateMarkHalfDayDeduction</t>
+  </si>
+  <si>
+    <t xml:space="preserve">80</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Check Leave deductions when Second Half leave is applied and approved for Late Mark Half day deduction</t>
+  </si>
+  <si>
+    <t xml:space="preserve">com.darwinbox.attendance.leavedeductions.latemark.halfday.TestSecondHalfAppliedAndApprovedForLateMarkHalfDayDeduction</t>
+  </si>
+  <si>
+    <t xml:space="preserve">81</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Check Leave deductions when Second Half leave is applied and pending for Late Mark Half day deduction</t>
+  </si>
+  <si>
+    <t xml:space="preserve">com.darwinbox.attendance.leavedeductions.latemark.halfday.TestSecondHalfAppliedAndPendingForLateMarkHalfDayDeduction</t>
+  </si>
+  <si>
+    <t xml:space="preserve">82</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Check Leave deductions when Full Day leave is applied and approved for Late Mark Half day deduction</t>
+  </si>
+  <si>
+    <t xml:space="preserve">com.darwinbox.attendance.leavedeductions.latemark.halfday.TestFullDayAppliedAndApprovedForLateMarkHalfDayDeduction</t>
+  </si>
+  <si>
+    <t xml:space="preserve">83</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Check Leave deductions when Full Day leave is applied and pending for Late Mark Half day deduction</t>
+  </si>
+  <si>
+    <t xml:space="preserve">com.darwinbox.attendance.leavedeductions.latemark.halfday.TestFullDayAppliedAndPendingForLateMarkHalfDayDeduction</t>
+  </si>
+  <si>
+    <t xml:space="preserve">84</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Check Leave deductions when no leave is applied for Late Mark Half day deduction</t>
+  </si>
+  <si>
+    <t xml:space="preserve">com.darwinbox.attendance.leavedeductions.latemark.halfday.TestForLateMarkHalfDayDeduction</t>
   </si>
 </sst>
 </file>
@@ -833,10 +968,10 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:J71"/>
+  <dimension ref="A1:J1048576"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="G1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="J1" activeCellId="0" sqref="J1"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A66" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="A72" activeCellId="0" sqref="A72"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15.75" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -1553,12 +1688,12 @@
         <v>18</v>
       </c>
       <c r="J22" s="0" t="s">
-        <v>83</v>
+        <v>19</v>
       </c>
     </row>
     <row r="23" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A23" s="0" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="B23" s="0" t="s">
         <v>11</v>
@@ -1570,10 +1705,10 @@
         <v>13</v>
       </c>
       <c r="E23" s="0" t="s">
+        <v>84</v>
+      </c>
+      <c r="F23" s="0" t="s">
         <v>85</v>
-      </c>
-      <c r="F23" s="0" t="s">
-        <v>86</v>
       </c>
       <c r="G23" s="0" t="s">
         <v>16</v>
@@ -1590,7 +1725,7 @@
     </row>
     <row r="24" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A24" s="0" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="B24" s="0" t="s">
         <v>11</v>
@@ -1602,10 +1737,10 @@
         <v>13</v>
       </c>
       <c r="E24" s="0" t="s">
+        <v>87</v>
+      </c>
+      <c r="F24" s="0" t="s">
         <v>88</v>
-      </c>
-      <c r="F24" s="0" t="s">
-        <v>89</v>
       </c>
       <c r="G24" s="0" t="s">
         <v>16</v>
@@ -1622,7 +1757,7 @@
     </row>
     <row r="25" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A25" s="0" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="B25" s="0" t="s">
         <v>11</v>
@@ -1634,10 +1769,10 @@
         <v>13</v>
       </c>
       <c r="E25" s="0" t="s">
+        <v>90</v>
+      </c>
+      <c r="F25" s="0" t="s">
         <v>91</v>
-      </c>
-      <c r="F25" s="0" t="s">
-        <v>92</v>
       </c>
       <c r="G25" s="0" t="s">
         <v>16</v>
@@ -1654,7 +1789,7 @@
     </row>
     <row r="26" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A26" s="0" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="B26" s="0" t="s">
         <v>11</v>
@@ -1666,10 +1801,10 @@
         <v>13</v>
       </c>
       <c r="E26" s="0" t="s">
+        <v>93</v>
+      </c>
+      <c r="F26" s="0" t="s">
         <v>94</v>
-      </c>
-      <c r="F26" s="0" t="s">
-        <v>95</v>
       </c>
       <c r="G26" s="0" t="s">
         <v>16</v>
@@ -1686,7 +1821,7 @@
     </row>
     <row r="27" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A27" s="0" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
       <c r="B27" s="0" t="s">
         <v>11</v>
@@ -1698,10 +1833,10 @@
         <v>13</v>
       </c>
       <c r="E27" s="0" t="s">
+        <v>96</v>
+      </c>
+      <c r="F27" s="0" t="s">
         <v>97</v>
-      </c>
-      <c r="F27" s="0" t="s">
-        <v>98</v>
       </c>
       <c r="G27" s="0" t="s">
         <v>16</v>
@@ -1718,7 +1853,7 @@
     </row>
     <row r="28" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A28" s="0" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
       <c r="B28" s="0" t="s">
         <v>11</v>
@@ -1730,10 +1865,10 @@
         <v>13</v>
       </c>
       <c r="E28" s="0" t="s">
+        <v>99</v>
+      </c>
+      <c r="F28" s="0" t="s">
         <v>100</v>
-      </c>
-      <c r="F28" s="0" t="s">
-        <v>101</v>
       </c>
       <c r="G28" s="0" t="s">
         <v>16</v>
@@ -1750,7 +1885,7 @@
     </row>
     <row r="29" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A29" s="0" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="B29" s="0" t="s">
         <v>11</v>
@@ -1762,10 +1897,10 @@
         <v>36</v>
       </c>
       <c r="E29" s="0" t="s">
+        <v>102</v>
+      </c>
+      <c r="F29" s="0" t="s">
         <v>103</v>
-      </c>
-      <c r="F29" s="0" t="s">
-        <v>104</v>
       </c>
       <c r="G29" s="0" t="s">
         <v>16</v>
@@ -1777,33 +1912,33 @@
         <v>18</v>
       </c>
       <c r="J29" s="0" t="s">
-        <v>83</v>
+        <v>19</v>
       </c>
     </row>
     <row r="30" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A30" s="0" t="s">
+        <v>104</v>
+      </c>
+      <c r="B30" s="0" t="s">
+        <v>11</v>
+      </c>
+      <c r="C30" s="0" t="s">
         <v>105</v>
       </c>
-      <c r="B30" s="0" t="s">
-        <v>11</v>
-      </c>
-      <c r="C30" s="0" t="s">
+      <c r="D30" s="0" t="s">
+        <v>13</v>
+      </c>
+      <c r="E30" s="0" t="s">
         <v>106</v>
       </c>
-      <c r="D30" s="0" t="s">
-        <v>13</v>
-      </c>
-      <c r="E30" s="0" t="s">
+      <c r="F30" s="0" t="s">
         <v>107</v>
       </c>
-      <c r="F30" s="0" t="s">
-        <v>108</v>
-      </c>
       <c r="G30" s="0" t="s">
         <v>16</v>
       </c>
       <c r="H30" s="0" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
       <c r="I30" s="0" t="s">
         <v>18</v>
@@ -1814,28 +1949,28 @@
     </row>
     <row r="31" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A31" s="0" t="s">
+        <v>108</v>
+      </c>
+      <c r="B31" s="0" t="s">
+        <v>11</v>
+      </c>
+      <c r="C31" s="0" t="s">
+        <v>105</v>
+      </c>
+      <c r="D31" s="0" t="s">
+        <v>13</v>
+      </c>
+      <c r="E31" s="0" t="s">
         <v>109</v>
       </c>
-      <c r="B31" s="0" t="s">
-        <v>11</v>
-      </c>
-      <c r="C31" s="0" t="s">
-        <v>106</v>
-      </c>
-      <c r="D31" s="0" t="s">
-        <v>13</v>
-      </c>
-      <c r="E31" s="0" t="s">
+      <c r="F31" s="0" t="s">
         <v>110</v>
       </c>
-      <c r="F31" s="0" t="s">
-        <v>111</v>
-      </c>
       <c r="G31" s="0" t="s">
         <v>16</v>
       </c>
       <c r="H31" s="0" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
       <c r="I31" s="0" t="s">
         <v>18</v>
@@ -1846,28 +1981,28 @@
     </row>
     <row r="32" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A32" s="0" t="s">
+        <v>111</v>
+      </c>
+      <c r="B32" s="0" t="s">
+        <v>11</v>
+      </c>
+      <c r="C32" s="0" t="s">
+        <v>105</v>
+      </c>
+      <c r="D32" s="0" t="s">
+        <v>13</v>
+      </c>
+      <c r="E32" s="0" t="s">
         <v>112</v>
       </c>
-      <c r="B32" s="0" t="s">
-        <v>11</v>
-      </c>
-      <c r="C32" s="0" t="s">
-        <v>106</v>
-      </c>
-      <c r="D32" s="0" t="s">
-        <v>13</v>
-      </c>
-      <c r="E32" s="0" t="s">
+      <c r="F32" s="0" t="s">
         <v>113</v>
       </c>
-      <c r="F32" s="0" t="s">
-        <v>114</v>
-      </c>
       <c r="G32" s="0" t="s">
         <v>16</v>
       </c>
       <c r="H32" s="0" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
       <c r="I32" s="0" t="s">
         <v>18</v>
@@ -1878,28 +2013,28 @@
     </row>
     <row r="33" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A33" s="0" t="s">
+        <v>114</v>
+      </c>
+      <c r="B33" s="0" t="s">
+        <v>11</v>
+      </c>
+      <c r="C33" s="0" t="s">
+        <v>105</v>
+      </c>
+      <c r="D33" s="0" t="s">
+        <v>13</v>
+      </c>
+      <c r="E33" s="0" t="s">
         <v>115</v>
       </c>
-      <c r="B33" s="0" t="s">
-        <v>11</v>
-      </c>
-      <c r="C33" s="0" t="s">
-        <v>106</v>
-      </c>
-      <c r="D33" s="0" t="s">
-        <v>13</v>
-      </c>
-      <c r="E33" s="0" t="s">
+      <c r="F33" s="0" t="s">
         <v>116</v>
       </c>
-      <c r="F33" s="0" t="s">
-        <v>117</v>
-      </c>
       <c r="G33" s="0" t="s">
         <v>16</v>
       </c>
       <c r="H33" s="0" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
       <c r="I33" s="0" t="s">
         <v>18</v>
@@ -1910,28 +2045,28 @@
     </row>
     <row r="34" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A34" s="0" t="s">
+        <v>117</v>
+      </c>
+      <c r="B34" s="0" t="s">
+        <v>11</v>
+      </c>
+      <c r="C34" s="0" t="s">
+        <v>105</v>
+      </c>
+      <c r="D34" s="0" t="s">
+        <v>13</v>
+      </c>
+      <c r="E34" s="0" t="s">
         <v>118</v>
       </c>
-      <c r="B34" s="0" t="s">
-        <v>11</v>
-      </c>
-      <c r="C34" s="0" t="s">
-        <v>106</v>
-      </c>
-      <c r="D34" s="0" t="s">
-        <v>13</v>
-      </c>
-      <c r="E34" s="0" t="s">
+      <c r="F34" s="0" t="s">
         <v>119</v>
       </c>
-      <c r="F34" s="0" t="s">
-        <v>120</v>
-      </c>
       <c r="G34" s="0" t="s">
         <v>16</v>
       </c>
       <c r="H34" s="0" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
       <c r="I34" s="0" t="s">
         <v>18</v>
@@ -1942,28 +2077,28 @@
     </row>
     <row r="35" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A35" s="0" t="s">
+        <v>120</v>
+      </c>
+      <c r="B35" s="0" t="s">
+        <v>11</v>
+      </c>
+      <c r="C35" s="0" t="s">
+        <v>105</v>
+      </c>
+      <c r="D35" s="0" t="s">
+        <v>13</v>
+      </c>
+      <c r="E35" s="0" t="s">
         <v>121</v>
       </c>
-      <c r="B35" s="0" t="s">
-        <v>11</v>
-      </c>
-      <c r="C35" s="0" t="s">
-        <v>106</v>
-      </c>
-      <c r="D35" s="0" t="s">
-        <v>13</v>
-      </c>
-      <c r="E35" s="0" t="s">
+      <c r="F35" s="0" t="s">
         <v>122</v>
       </c>
-      <c r="F35" s="0" t="s">
-        <v>123</v>
-      </c>
       <c r="G35" s="0" t="s">
         <v>16</v>
       </c>
       <c r="H35" s="0" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
       <c r="I35" s="0" t="s">
         <v>18</v>
@@ -1974,60 +2109,60 @@
     </row>
     <row r="36" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A36" s="0" t="s">
-        <v>124</v>
+        <v>123</v>
       </c>
       <c r="B36" s="0" t="s">
         <v>11</v>
       </c>
       <c r="C36" s="0" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
       <c r="D36" s="0" t="s">
         <v>36</v>
       </c>
       <c r="E36" s="0" t="s">
+        <v>124</v>
+      </c>
+      <c r="F36" s="0" t="s">
         <v>125</v>
       </c>
-      <c r="F36" s="0" t="s">
-        <v>126</v>
-      </c>
       <c r="G36" s="0" t="s">
         <v>16</v>
       </c>
       <c r="H36" s="0" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
       <c r="I36" s="0" t="s">
         <v>18</v>
       </c>
       <c r="J36" s="0" t="s">
-        <v>83</v>
+        <v>19</v>
       </c>
     </row>
     <row r="37" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A37" s="0" t="s">
+        <v>126</v>
+      </c>
+      <c r="B37" s="0" t="s">
+        <v>11</v>
+      </c>
+      <c r="C37" s="0" t="s">
+        <v>105</v>
+      </c>
+      <c r="D37" s="0" t="s">
+        <v>13</v>
+      </c>
+      <c r="E37" s="0" t="s">
         <v>127</v>
       </c>
-      <c r="B37" s="0" t="s">
-        <v>11</v>
-      </c>
-      <c r="C37" s="0" t="s">
-        <v>106</v>
-      </c>
-      <c r="D37" s="0" t="s">
-        <v>13</v>
-      </c>
-      <c r="E37" s="0" t="s">
+      <c r="F37" s="0" t="s">
         <v>128</v>
       </c>
-      <c r="F37" s="0" t="s">
-        <v>129</v>
-      </c>
       <c r="G37" s="0" t="s">
         <v>16</v>
       </c>
       <c r="H37" s="0" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
       <c r="I37" s="0" t="s">
         <v>18</v>
@@ -2038,28 +2173,28 @@
     </row>
     <row r="38" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A38" s="0" t="s">
+        <v>129</v>
+      </c>
+      <c r="B38" s="0" t="s">
+        <v>11</v>
+      </c>
+      <c r="C38" s="0" t="s">
+        <v>105</v>
+      </c>
+      <c r="D38" s="0" t="s">
+        <v>13</v>
+      </c>
+      <c r="E38" s="0" t="s">
         <v>130</v>
       </c>
-      <c r="B38" s="0" t="s">
-        <v>11</v>
-      </c>
-      <c r="C38" s="0" t="s">
-        <v>106</v>
-      </c>
-      <c r="D38" s="0" t="s">
-        <v>13</v>
-      </c>
-      <c r="E38" s="0" t="s">
+      <c r="F38" s="0" t="s">
         <v>131</v>
       </c>
-      <c r="F38" s="0" t="s">
-        <v>132</v>
-      </c>
       <c r="G38" s="0" t="s">
         <v>16</v>
       </c>
       <c r="H38" s="0" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
       <c r="I38" s="0" t="s">
         <v>18</v>
@@ -2070,28 +2205,28 @@
     </row>
     <row r="39" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A39" s="0" t="s">
+        <v>132</v>
+      </c>
+      <c r="B39" s="0" t="s">
+        <v>11</v>
+      </c>
+      <c r="C39" s="0" t="s">
+        <v>105</v>
+      </c>
+      <c r="D39" s="0" t="s">
+        <v>13</v>
+      </c>
+      <c r="E39" s="0" t="s">
         <v>133</v>
       </c>
-      <c r="B39" s="0" t="s">
-        <v>11</v>
-      </c>
-      <c r="C39" s="0" t="s">
-        <v>106</v>
-      </c>
-      <c r="D39" s="0" t="s">
-        <v>13</v>
-      </c>
-      <c r="E39" s="0" t="s">
+      <c r="F39" s="0" t="s">
         <v>134</v>
       </c>
-      <c r="F39" s="0" t="s">
-        <v>135</v>
-      </c>
       <c r="G39" s="0" t="s">
         <v>16</v>
       </c>
       <c r="H39" s="0" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
       <c r="I39" s="0" t="s">
         <v>18</v>
@@ -2102,28 +2237,28 @@
     </row>
     <row r="40" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A40" s="0" t="s">
+        <v>135</v>
+      </c>
+      <c r="B40" s="0" t="s">
+        <v>11</v>
+      </c>
+      <c r="C40" s="0" t="s">
+        <v>105</v>
+      </c>
+      <c r="D40" s="0" t="s">
+        <v>13</v>
+      </c>
+      <c r="E40" s="0" t="s">
         <v>136</v>
       </c>
-      <c r="B40" s="0" t="s">
-        <v>11</v>
-      </c>
-      <c r="C40" s="0" t="s">
-        <v>106</v>
-      </c>
-      <c r="D40" s="0" t="s">
-        <v>13</v>
-      </c>
-      <c r="E40" s="0" t="s">
+      <c r="F40" s="0" t="s">
         <v>137</v>
       </c>
-      <c r="F40" s="0" t="s">
-        <v>138</v>
-      </c>
       <c r="G40" s="0" t="s">
         <v>16</v>
       </c>
       <c r="H40" s="0" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
       <c r="I40" s="0" t="s">
         <v>18</v>
@@ -2134,28 +2269,28 @@
     </row>
     <row r="41" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A41" s="0" t="s">
+        <v>138</v>
+      </c>
+      <c r="B41" s="0" t="s">
+        <v>11</v>
+      </c>
+      <c r="C41" s="0" t="s">
+        <v>105</v>
+      </c>
+      <c r="D41" s="0" t="s">
+        <v>13</v>
+      </c>
+      <c r="E41" s="0" t="s">
         <v>139</v>
       </c>
-      <c r="B41" s="0" t="s">
-        <v>11</v>
-      </c>
-      <c r="C41" s="0" t="s">
-        <v>106</v>
-      </c>
-      <c r="D41" s="0" t="s">
-        <v>13</v>
-      </c>
-      <c r="E41" s="0" t="s">
+      <c r="F41" s="0" t="s">
         <v>140</v>
       </c>
-      <c r="F41" s="0" t="s">
-        <v>141</v>
-      </c>
       <c r="G41" s="0" t="s">
         <v>16</v>
       </c>
       <c r="H41" s="0" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
       <c r="I41" s="0" t="s">
         <v>18</v>
@@ -2166,28 +2301,28 @@
     </row>
     <row r="42" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A42" s="0" t="s">
+        <v>141</v>
+      </c>
+      <c r="B42" s="0" t="s">
+        <v>11</v>
+      </c>
+      <c r="C42" s="0" t="s">
+        <v>105</v>
+      </c>
+      <c r="D42" s="0" t="s">
+        <v>13</v>
+      </c>
+      <c r="E42" s="0" t="s">
         <v>142</v>
       </c>
-      <c r="B42" s="0" t="s">
-        <v>11</v>
-      </c>
-      <c r="C42" s="0" t="s">
-        <v>106</v>
-      </c>
-      <c r="D42" s="0" t="s">
-        <v>13</v>
-      </c>
-      <c r="E42" s="0" t="s">
+      <c r="F42" s="0" t="s">
         <v>143</v>
       </c>
-      <c r="F42" s="0" t="s">
-        <v>144</v>
-      </c>
       <c r="G42" s="0" t="s">
         <v>16</v>
       </c>
       <c r="H42" s="0" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
       <c r="I42" s="0" t="s">
         <v>18</v>
@@ -2198,60 +2333,60 @@
     </row>
     <row r="43" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A43" s="0" t="s">
-        <v>145</v>
+        <v>144</v>
       </c>
       <c r="B43" s="0" t="s">
         <v>11</v>
       </c>
       <c r="C43" s="0" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
       <c r="D43" s="0" t="s">
         <v>36</v>
       </c>
       <c r="E43" s="0" t="s">
+        <v>145</v>
+      </c>
+      <c r="F43" s="0" t="s">
         <v>146</v>
       </c>
-      <c r="F43" s="0" t="s">
-        <v>147</v>
-      </c>
       <c r="G43" s="0" t="s">
         <v>16</v>
       </c>
       <c r="H43" s="0" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
       <c r="I43" s="0" t="s">
         <v>18</v>
       </c>
       <c r="J43" s="0" t="s">
-        <v>83</v>
+        <v>19</v>
       </c>
     </row>
     <row r="44" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A44" s="0" t="s">
+        <v>147</v>
+      </c>
+      <c r="B44" s="0" t="s">
+        <v>11</v>
+      </c>
+      <c r="C44" s="0" t="s">
         <v>148</v>
       </c>
-      <c r="B44" s="0" t="s">
-        <v>11</v>
-      </c>
-      <c r="C44" s="0" t="s">
+      <c r="D44" s="0" t="s">
+        <v>13</v>
+      </c>
+      <c r="E44" s="0" t="s">
         <v>149</v>
       </c>
-      <c r="D44" s="0" t="s">
-        <v>13</v>
-      </c>
-      <c r="E44" s="0" t="s">
+      <c r="F44" s="0" t="s">
         <v>150</v>
       </c>
-      <c r="F44" s="0" t="s">
-        <v>151</v>
-      </c>
       <c r="G44" s="0" t="s">
         <v>16</v>
       </c>
       <c r="H44" s="0" t="s">
-        <v>149</v>
+        <v>148</v>
       </c>
       <c r="I44" s="0" t="s">
         <v>18</v>
@@ -2262,28 +2397,28 @@
     </row>
     <row r="45" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A45" s="0" t="s">
+        <v>151</v>
+      </c>
+      <c r="B45" s="0" t="s">
+        <v>11</v>
+      </c>
+      <c r="C45" s="0" t="s">
+        <v>148</v>
+      </c>
+      <c r="D45" s="0" t="s">
+        <v>13</v>
+      </c>
+      <c r="E45" s="0" t="s">
         <v>152</v>
       </c>
-      <c r="B45" s="0" t="s">
-        <v>11</v>
-      </c>
-      <c r="C45" s="0" t="s">
-        <v>149</v>
-      </c>
-      <c r="D45" s="0" t="s">
-        <v>13</v>
-      </c>
-      <c r="E45" s="0" t="s">
+      <c r="F45" s="0" t="s">
         <v>153</v>
       </c>
-      <c r="F45" s="0" t="s">
-        <v>154</v>
-      </c>
       <c r="G45" s="0" t="s">
         <v>16</v>
       </c>
       <c r="H45" s="0" t="s">
-        <v>149</v>
+        <v>148</v>
       </c>
       <c r="I45" s="0" t="s">
         <v>18</v>
@@ -2294,28 +2429,28 @@
     </row>
     <row r="46" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A46" s="0" t="s">
+        <v>154</v>
+      </c>
+      <c r="B46" s="0" t="s">
+        <v>11</v>
+      </c>
+      <c r="C46" s="0" t="s">
+        <v>148</v>
+      </c>
+      <c r="D46" s="0" t="s">
+        <v>13</v>
+      </c>
+      <c r="E46" s="0" t="s">
         <v>155</v>
       </c>
-      <c r="B46" s="0" t="s">
-        <v>11</v>
-      </c>
-      <c r="C46" s="0" t="s">
-        <v>149</v>
-      </c>
-      <c r="D46" s="0" t="s">
-        <v>13</v>
-      </c>
-      <c r="E46" s="0" t="s">
+      <c r="F46" s="0" t="s">
         <v>156</v>
       </c>
-      <c r="F46" s="0" t="s">
-        <v>157</v>
-      </c>
       <c r="G46" s="0" t="s">
         <v>16</v>
       </c>
       <c r="H46" s="0" t="s">
-        <v>149</v>
+        <v>148</v>
       </c>
       <c r="I46" s="0" t="s">
         <v>18</v>
@@ -2326,28 +2461,28 @@
     </row>
     <row r="47" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A47" s="0" t="s">
+        <v>157</v>
+      </c>
+      <c r="B47" s="0" t="s">
+        <v>11</v>
+      </c>
+      <c r="C47" s="0" t="s">
+        <v>148</v>
+      </c>
+      <c r="D47" s="0" t="s">
+        <v>13</v>
+      </c>
+      <c r="E47" s="0" t="s">
         <v>158</v>
       </c>
-      <c r="B47" s="0" t="s">
-        <v>11</v>
-      </c>
-      <c r="C47" s="0" t="s">
-        <v>149</v>
-      </c>
-      <c r="D47" s="0" t="s">
-        <v>13</v>
-      </c>
-      <c r="E47" s="0" t="s">
+      <c r="F47" s="0" t="s">
         <v>159</v>
       </c>
-      <c r="F47" s="0" t="s">
-        <v>160</v>
-      </c>
       <c r="G47" s="0" t="s">
         <v>16</v>
       </c>
       <c r="H47" s="0" t="s">
-        <v>149</v>
+        <v>148</v>
       </c>
       <c r="I47" s="0" t="s">
         <v>18</v>
@@ -2358,28 +2493,28 @@
     </row>
     <row r="48" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A48" s="0" t="s">
+        <v>160</v>
+      </c>
+      <c r="B48" s="0" t="s">
+        <v>11</v>
+      </c>
+      <c r="C48" s="0" t="s">
+        <v>148</v>
+      </c>
+      <c r="D48" s="0" t="s">
+        <v>13</v>
+      </c>
+      <c r="E48" s="0" t="s">
         <v>161</v>
       </c>
-      <c r="B48" s="0" t="s">
-        <v>11</v>
-      </c>
-      <c r="C48" s="0" t="s">
-        <v>149</v>
-      </c>
-      <c r="D48" s="0" t="s">
-        <v>13</v>
-      </c>
-      <c r="E48" s="0" t="s">
+      <c r="F48" s="0" t="s">
         <v>162</v>
       </c>
-      <c r="F48" s="0" t="s">
-        <v>163</v>
-      </c>
       <c r="G48" s="0" t="s">
         <v>16</v>
       </c>
       <c r="H48" s="0" t="s">
-        <v>149</v>
+        <v>148</v>
       </c>
       <c r="I48" s="0" t="s">
         <v>18</v>
@@ -2390,28 +2525,28 @@
     </row>
     <row r="49" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A49" s="0" t="s">
+        <v>163</v>
+      </c>
+      <c r="B49" s="0" t="s">
+        <v>11</v>
+      </c>
+      <c r="C49" s="0" t="s">
+        <v>148</v>
+      </c>
+      <c r="D49" s="0" t="s">
+        <v>13</v>
+      </c>
+      <c r="E49" s="0" t="s">
         <v>164</v>
       </c>
-      <c r="B49" s="0" t="s">
-        <v>11</v>
-      </c>
-      <c r="C49" s="0" t="s">
-        <v>149</v>
-      </c>
-      <c r="D49" s="0" t="s">
-        <v>13</v>
-      </c>
-      <c r="E49" s="0" t="s">
+      <c r="F49" s="0" t="s">
         <v>165</v>
       </c>
-      <c r="F49" s="0" t="s">
-        <v>166</v>
-      </c>
       <c r="G49" s="0" t="s">
         <v>16</v>
       </c>
       <c r="H49" s="0" t="s">
-        <v>149</v>
+        <v>148</v>
       </c>
       <c r="I49" s="0" t="s">
         <v>18</v>
@@ -2422,60 +2557,60 @@
     </row>
     <row r="50" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A50" s="0" t="s">
-        <v>167</v>
+        <v>166</v>
       </c>
       <c r="B50" s="0" t="s">
         <v>11</v>
       </c>
       <c r="C50" s="0" t="s">
-        <v>149</v>
+        <v>148</v>
       </c>
       <c r="D50" s="0" t="s">
         <v>36</v>
       </c>
       <c r="E50" s="0" t="s">
+        <v>167</v>
+      </c>
+      <c r="F50" s="0" t="s">
         <v>168</v>
       </c>
-      <c r="F50" s="0" t="s">
-        <v>169</v>
-      </c>
       <c r="G50" s="0" t="s">
         <v>16</v>
       </c>
       <c r="H50" s="0" t="s">
-        <v>149</v>
+        <v>148</v>
       </c>
       <c r="I50" s="0" t="s">
         <v>18</v>
       </c>
       <c r="J50" s="0" t="s">
-        <v>83</v>
+        <v>19</v>
       </c>
     </row>
     <row r="51" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A51" s="0" t="s">
+        <v>169</v>
+      </c>
+      <c r="B51" s="0" t="s">
+        <v>11</v>
+      </c>
+      <c r="C51" s="0" t="s">
+        <v>148</v>
+      </c>
+      <c r="D51" s="0" t="s">
+        <v>13</v>
+      </c>
+      <c r="E51" s="0" t="s">
         <v>170</v>
       </c>
-      <c r="B51" s="0" t="s">
-        <v>11</v>
-      </c>
-      <c r="C51" s="0" t="s">
-        <v>149</v>
-      </c>
-      <c r="D51" s="0" t="s">
-        <v>13</v>
-      </c>
-      <c r="E51" s="0" t="s">
+      <c r="F51" s="0" t="s">
         <v>171</v>
       </c>
-      <c r="F51" s="0" t="s">
-        <v>172</v>
-      </c>
       <c r="G51" s="0" t="s">
         <v>16</v>
       </c>
       <c r="H51" s="0" t="s">
-        <v>149</v>
+        <v>148</v>
       </c>
       <c r="I51" s="0" t="s">
         <v>18</v>
@@ -2486,28 +2621,28 @@
     </row>
     <row r="52" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A52" s="0" t="s">
+        <v>172</v>
+      </c>
+      <c r="B52" s="0" t="s">
+        <v>11</v>
+      </c>
+      <c r="C52" s="0" t="s">
+        <v>148</v>
+      </c>
+      <c r="D52" s="0" t="s">
+        <v>13</v>
+      </c>
+      <c r="E52" s="0" t="s">
         <v>173</v>
       </c>
-      <c r="B52" s="0" t="s">
-        <v>11</v>
-      </c>
-      <c r="C52" s="0" t="s">
-        <v>149</v>
-      </c>
-      <c r="D52" s="0" t="s">
-        <v>13</v>
-      </c>
-      <c r="E52" s="0" t="s">
+      <c r="F52" s="0" t="s">
         <v>174</v>
       </c>
-      <c r="F52" s="0" t="s">
-        <v>175</v>
-      </c>
       <c r="G52" s="0" t="s">
         <v>16</v>
       </c>
       <c r="H52" s="0" t="s">
-        <v>149</v>
+        <v>148</v>
       </c>
       <c r="I52" s="0" t="s">
         <v>18</v>
@@ -2518,28 +2653,28 @@
     </row>
     <row r="53" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A53" s="0" t="s">
+        <v>175</v>
+      </c>
+      <c r="B53" s="0" t="s">
+        <v>11</v>
+      </c>
+      <c r="C53" s="0" t="s">
+        <v>148</v>
+      </c>
+      <c r="D53" s="0" t="s">
+        <v>13</v>
+      </c>
+      <c r="E53" s="0" t="s">
         <v>176</v>
       </c>
-      <c r="B53" s="0" t="s">
-        <v>11</v>
-      </c>
-      <c r="C53" s="0" t="s">
-        <v>149</v>
-      </c>
-      <c r="D53" s="0" t="s">
-        <v>13</v>
-      </c>
-      <c r="E53" s="0" t="s">
+      <c r="F53" s="0" t="s">
         <v>177</v>
       </c>
-      <c r="F53" s="0" t="s">
-        <v>178</v>
-      </c>
       <c r="G53" s="0" t="s">
         <v>16</v>
       </c>
       <c r="H53" s="0" t="s">
-        <v>149</v>
+        <v>148</v>
       </c>
       <c r="I53" s="0" t="s">
         <v>18</v>
@@ -2550,28 +2685,28 @@
     </row>
     <row r="54" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A54" s="0" t="s">
+        <v>178</v>
+      </c>
+      <c r="B54" s="0" t="s">
+        <v>11</v>
+      </c>
+      <c r="C54" s="0" t="s">
+        <v>148</v>
+      </c>
+      <c r="D54" s="0" t="s">
+        <v>13</v>
+      </c>
+      <c r="E54" s="0" t="s">
         <v>179</v>
       </c>
-      <c r="B54" s="0" t="s">
-        <v>11</v>
-      </c>
-      <c r="C54" s="0" t="s">
-        <v>149</v>
-      </c>
-      <c r="D54" s="0" t="s">
-        <v>13</v>
-      </c>
-      <c r="E54" s="0" t="s">
+      <c r="F54" s="0" t="s">
         <v>180</v>
       </c>
-      <c r="F54" s="0" t="s">
-        <v>181</v>
-      </c>
       <c r="G54" s="0" t="s">
         <v>16</v>
       </c>
       <c r="H54" s="0" t="s">
-        <v>149</v>
+        <v>148</v>
       </c>
       <c r="I54" s="0" t="s">
         <v>18</v>
@@ -2582,28 +2717,28 @@
     </row>
     <row r="55" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A55" s="0" t="s">
+        <v>181</v>
+      </c>
+      <c r="B55" s="0" t="s">
+        <v>11</v>
+      </c>
+      <c r="C55" s="0" t="s">
+        <v>148</v>
+      </c>
+      <c r="D55" s="0" t="s">
+        <v>13</v>
+      </c>
+      <c r="E55" s="0" t="s">
         <v>182</v>
       </c>
-      <c r="B55" s="0" t="s">
-        <v>11</v>
-      </c>
-      <c r="C55" s="0" t="s">
-        <v>149</v>
-      </c>
-      <c r="D55" s="0" t="s">
-        <v>13</v>
-      </c>
-      <c r="E55" s="0" t="s">
+      <c r="F55" s="0" t="s">
         <v>183</v>
       </c>
-      <c r="F55" s="0" t="s">
-        <v>184</v>
-      </c>
       <c r="G55" s="0" t="s">
         <v>16</v>
       </c>
       <c r="H55" s="0" t="s">
-        <v>149</v>
+        <v>148</v>
       </c>
       <c r="I55" s="0" t="s">
         <v>18</v>
@@ -2614,28 +2749,28 @@
     </row>
     <row r="56" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A56" s="0" t="s">
+        <v>184</v>
+      </c>
+      <c r="B56" s="0" t="s">
+        <v>11</v>
+      </c>
+      <c r="C56" s="0" t="s">
+        <v>148</v>
+      </c>
+      <c r="D56" s="0" t="s">
+        <v>13</v>
+      </c>
+      <c r="E56" s="0" t="s">
         <v>185</v>
       </c>
-      <c r="B56" s="0" t="s">
-        <v>11</v>
-      </c>
-      <c r="C56" s="0" t="s">
-        <v>149</v>
-      </c>
-      <c r="D56" s="0" t="s">
-        <v>13</v>
-      </c>
-      <c r="E56" s="0" t="s">
+      <c r="F56" s="0" t="s">
         <v>186</v>
       </c>
-      <c r="F56" s="0" t="s">
-        <v>187</v>
-      </c>
       <c r="G56" s="0" t="s">
         <v>16</v>
       </c>
       <c r="H56" s="0" t="s">
-        <v>149</v>
+        <v>148</v>
       </c>
       <c r="I56" s="0" t="s">
         <v>18</v>
@@ -2646,60 +2781,60 @@
     </row>
     <row r="57" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A57" s="0" t="s">
-        <v>188</v>
+        <v>187</v>
       </c>
       <c r="B57" s="0" t="s">
         <v>11</v>
       </c>
       <c r="C57" s="0" t="s">
-        <v>149</v>
+        <v>148</v>
       </c>
       <c r="D57" s="0" t="s">
         <v>36</v>
       </c>
       <c r="E57" s="0" t="s">
+        <v>188</v>
+      </c>
+      <c r="F57" s="0" t="s">
         <v>189</v>
       </c>
-      <c r="F57" s="0" t="s">
-        <v>190</v>
-      </c>
       <c r="G57" s="0" t="s">
         <v>16</v>
       </c>
       <c r="H57" s="0" t="s">
-        <v>149</v>
+        <v>148</v>
       </c>
       <c r="I57" s="0" t="s">
         <v>18</v>
       </c>
       <c r="J57" s="0" t="s">
-        <v>83</v>
+        <v>19</v>
       </c>
     </row>
     <row r="58" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A58" s="0" t="s">
+        <v>190</v>
+      </c>
+      <c r="B58" s="0" t="s">
+        <v>11</v>
+      </c>
+      <c r="C58" s="0" t="s">
         <v>191</v>
       </c>
-      <c r="B58" s="0" t="s">
-        <v>11</v>
-      </c>
-      <c r="C58" s="0" t="s">
+      <c r="D58" s="0" t="s">
+        <v>13</v>
+      </c>
+      <c r="E58" s="0" t="s">
         <v>192</v>
       </c>
-      <c r="D58" s="0" t="s">
-        <v>13</v>
-      </c>
-      <c r="E58" s="0" t="s">
+      <c r="F58" s="0" t="s">
         <v>193</v>
       </c>
-      <c r="F58" s="0" t="s">
-        <v>194</v>
-      </c>
       <c r="G58" s="0" t="s">
         <v>16</v>
       </c>
       <c r="H58" s="0" t="s">
-        <v>192</v>
+        <v>191</v>
       </c>
       <c r="I58" s="0" t="s">
         <v>18</v>
@@ -2710,28 +2845,28 @@
     </row>
     <row r="59" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A59" s="0" t="s">
+        <v>194</v>
+      </c>
+      <c r="B59" s="0" t="s">
+        <v>11</v>
+      </c>
+      <c r="C59" s="0" t="s">
+        <v>191</v>
+      </c>
+      <c r="D59" s="0" t="s">
+        <v>13</v>
+      </c>
+      <c r="E59" s="0" t="s">
         <v>195</v>
       </c>
-      <c r="B59" s="0" t="s">
-        <v>11</v>
-      </c>
-      <c r="C59" s="0" t="s">
-        <v>192</v>
-      </c>
-      <c r="D59" s="0" t="s">
-        <v>13</v>
-      </c>
-      <c r="E59" s="0" t="s">
+      <c r="F59" s="0" t="s">
         <v>196</v>
       </c>
-      <c r="F59" s="0" t="s">
-        <v>197</v>
-      </c>
       <c r="G59" s="0" t="s">
         <v>16</v>
       </c>
       <c r="H59" s="0" t="s">
-        <v>192</v>
+        <v>191</v>
       </c>
       <c r="I59" s="0" t="s">
         <v>18</v>
@@ -2742,28 +2877,28 @@
     </row>
     <row r="60" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A60" s="0" t="s">
+        <v>197</v>
+      </c>
+      <c r="B60" s="0" t="s">
+        <v>11</v>
+      </c>
+      <c r="C60" s="0" t="s">
+        <v>191</v>
+      </c>
+      <c r="D60" s="0" t="s">
+        <v>13</v>
+      </c>
+      <c r="E60" s="0" t="s">
         <v>198</v>
       </c>
-      <c r="B60" s="0" t="s">
-        <v>11</v>
-      </c>
-      <c r="C60" s="0" t="s">
-        <v>192</v>
-      </c>
-      <c r="D60" s="0" t="s">
-        <v>13</v>
-      </c>
-      <c r="E60" s="0" t="s">
+      <c r="F60" s="0" t="s">
         <v>199</v>
       </c>
-      <c r="F60" s="0" t="s">
-        <v>200</v>
-      </c>
       <c r="G60" s="0" t="s">
         <v>16</v>
       </c>
       <c r="H60" s="0" t="s">
-        <v>192</v>
+        <v>191</v>
       </c>
       <c r="I60" s="0" t="s">
         <v>18</v>
@@ -2774,28 +2909,28 @@
     </row>
     <row r="61" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A61" s="0" t="s">
+        <v>200</v>
+      </c>
+      <c r="B61" s="0" t="s">
+        <v>11</v>
+      </c>
+      <c r="C61" s="0" t="s">
+        <v>191</v>
+      </c>
+      <c r="D61" s="0" t="s">
+        <v>13</v>
+      </c>
+      <c r="E61" s="0" t="s">
         <v>201</v>
       </c>
-      <c r="B61" s="0" t="s">
-        <v>11</v>
-      </c>
-      <c r="C61" s="0" t="s">
-        <v>192</v>
-      </c>
-      <c r="D61" s="0" t="s">
-        <v>13</v>
-      </c>
-      <c r="E61" s="0" t="s">
+      <c r="F61" s="0" t="s">
         <v>202</v>
       </c>
-      <c r="F61" s="0" t="s">
-        <v>203</v>
-      </c>
       <c r="G61" s="0" t="s">
         <v>16</v>
       </c>
       <c r="H61" s="0" t="s">
-        <v>192</v>
+        <v>191</v>
       </c>
       <c r="I61" s="0" t="s">
         <v>18</v>
@@ -2806,28 +2941,28 @@
     </row>
     <row r="62" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A62" s="0" t="s">
+        <v>203</v>
+      </c>
+      <c r="B62" s="0" t="s">
+        <v>11</v>
+      </c>
+      <c r="C62" s="0" t="s">
+        <v>191</v>
+      </c>
+      <c r="D62" s="0" t="s">
+        <v>13</v>
+      </c>
+      <c r="E62" s="0" t="s">
         <v>204</v>
       </c>
-      <c r="B62" s="0" t="s">
-        <v>11</v>
-      </c>
-      <c r="C62" s="0" t="s">
-        <v>192</v>
-      </c>
-      <c r="D62" s="0" t="s">
-        <v>13</v>
-      </c>
-      <c r="E62" s="0" t="s">
+      <c r="F62" s="0" t="s">
         <v>205</v>
       </c>
-      <c r="F62" s="0" t="s">
-        <v>206</v>
-      </c>
       <c r="G62" s="0" t="s">
         <v>16</v>
       </c>
       <c r="H62" s="0" t="s">
-        <v>192</v>
+        <v>191</v>
       </c>
       <c r="I62" s="0" t="s">
         <v>18</v>
@@ -2838,28 +2973,28 @@
     </row>
     <row r="63" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A63" s="0" t="s">
+        <v>206</v>
+      </c>
+      <c r="B63" s="0" t="s">
+        <v>11</v>
+      </c>
+      <c r="C63" s="0" t="s">
+        <v>191</v>
+      </c>
+      <c r="D63" s="0" t="s">
+        <v>13</v>
+      </c>
+      <c r="E63" s="0" t="s">
         <v>207</v>
       </c>
-      <c r="B63" s="0" t="s">
-        <v>11</v>
-      </c>
-      <c r="C63" s="0" t="s">
-        <v>192</v>
-      </c>
-      <c r="D63" s="0" t="s">
-        <v>13</v>
-      </c>
-      <c r="E63" s="0" t="s">
+      <c r="F63" s="0" t="s">
         <v>208</v>
       </c>
-      <c r="F63" s="0" t="s">
-        <v>209</v>
-      </c>
       <c r="G63" s="0" t="s">
         <v>16</v>
       </c>
       <c r="H63" s="0" t="s">
-        <v>192</v>
+        <v>191</v>
       </c>
       <c r="I63" s="0" t="s">
         <v>18</v>
@@ -2870,60 +3005,60 @@
     </row>
     <row r="64" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A64" s="0" t="s">
-        <v>210</v>
+        <v>209</v>
       </c>
       <c r="B64" s="0" t="s">
         <v>11</v>
       </c>
       <c r="C64" s="0" t="s">
-        <v>192</v>
+        <v>191</v>
       </c>
       <c r="D64" s="0" t="s">
         <v>36</v>
       </c>
       <c r="E64" s="0" t="s">
+        <v>210</v>
+      </c>
+      <c r="F64" s="0" t="s">
         <v>211</v>
       </c>
-      <c r="F64" s="0" t="s">
-        <v>212</v>
-      </c>
       <c r="G64" s="0" t="s">
         <v>16</v>
       </c>
       <c r="H64" s="0" t="s">
-        <v>192</v>
+        <v>191</v>
       </c>
       <c r="I64" s="0" t="s">
         <v>18</v>
       </c>
       <c r="J64" s="0" t="s">
-        <v>83</v>
+        <v>19</v>
       </c>
     </row>
     <row r="65" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A65" s="0" t="s">
+        <v>212</v>
+      </c>
+      <c r="B65" s="0" t="s">
+        <v>11</v>
+      </c>
+      <c r="C65" s="0" t="s">
+        <v>191</v>
+      </c>
+      <c r="D65" s="0" t="s">
+        <v>13</v>
+      </c>
+      <c r="E65" s="0" t="s">
         <v>213</v>
       </c>
-      <c r="B65" s="0" t="s">
-        <v>11</v>
-      </c>
-      <c r="C65" s="0" t="s">
-        <v>192</v>
-      </c>
-      <c r="D65" s="0" t="s">
-        <v>13</v>
-      </c>
-      <c r="E65" s="0" t="s">
+      <c r="F65" s="0" t="s">
         <v>214</v>
       </c>
-      <c r="F65" s="0" t="s">
-        <v>215</v>
-      </c>
       <c r="G65" s="0" t="s">
         <v>16</v>
       </c>
       <c r="H65" s="0" t="s">
-        <v>192</v>
+        <v>191</v>
       </c>
       <c r="I65" s="0" t="s">
         <v>18</v>
@@ -2934,28 +3069,28 @@
     </row>
     <row r="66" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A66" s="0" t="s">
+        <v>215</v>
+      </c>
+      <c r="B66" s="0" t="s">
+        <v>11</v>
+      </c>
+      <c r="C66" s="0" t="s">
+        <v>191</v>
+      </c>
+      <c r="D66" s="0" t="s">
+        <v>13</v>
+      </c>
+      <c r="E66" s="0" t="s">
         <v>216</v>
       </c>
-      <c r="B66" s="0" t="s">
-        <v>11</v>
-      </c>
-      <c r="C66" s="0" t="s">
-        <v>192</v>
-      </c>
-      <c r="D66" s="0" t="s">
-        <v>13</v>
-      </c>
-      <c r="E66" s="0" t="s">
+      <c r="F66" s="0" t="s">
         <v>217</v>
       </c>
-      <c r="F66" s="0" t="s">
-        <v>218</v>
-      </c>
       <c r="G66" s="0" t="s">
         <v>16</v>
       </c>
       <c r="H66" s="0" t="s">
-        <v>192</v>
+        <v>191</v>
       </c>
       <c r="I66" s="0" t="s">
         <v>18</v>
@@ -2966,28 +3101,28 @@
     </row>
     <row r="67" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A67" s="0" t="s">
+        <v>218</v>
+      </c>
+      <c r="B67" s="0" t="s">
+        <v>11</v>
+      </c>
+      <c r="C67" s="0" t="s">
+        <v>191</v>
+      </c>
+      <c r="D67" s="0" t="s">
+        <v>13</v>
+      </c>
+      <c r="E67" s="0" t="s">
         <v>219</v>
       </c>
-      <c r="B67" s="0" t="s">
-        <v>11</v>
-      </c>
-      <c r="C67" s="0" t="s">
-        <v>192</v>
-      </c>
-      <c r="D67" s="0" t="s">
-        <v>13</v>
-      </c>
-      <c r="E67" s="0" t="s">
+      <c r="F67" s="0" t="s">
         <v>220</v>
       </c>
-      <c r="F67" s="0" t="s">
-        <v>221</v>
-      </c>
       <c r="G67" s="0" t="s">
         <v>16</v>
       </c>
       <c r="H67" s="0" t="s">
-        <v>192</v>
+        <v>191</v>
       </c>
       <c r="I67" s="0" t="s">
         <v>18</v>
@@ -2998,28 +3133,28 @@
     </row>
     <row r="68" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A68" s="0" t="s">
+        <v>221</v>
+      </c>
+      <c r="B68" s="0" t="s">
+        <v>11</v>
+      </c>
+      <c r="C68" s="0" t="s">
+        <v>191</v>
+      </c>
+      <c r="D68" s="0" t="s">
+        <v>13</v>
+      </c>
+      <c r="E68" s="0" t="s">
         <v>222</v>
       </c>
-      <c r="B68" s="0" t="s">
-        <v>11</v>
-      </c>
-      <c r="C68" s="0" t="s">
-        <v>192</v>
-      </c>
-      <c r="D68" s="0" t="s">
-        <v>13</v>
-      </c>
-      <c r="E68" s="0" t="s">
+      <c r="F68" s="0" t="s">
         <v>223</v>
       </c>
-      <c r="F68" s="0" t="s">
-        <v>224</v>
-      </c>
       <c r="G68" s="0" t="s">
         <v>16</v>
       </c>
       <c r="H68" s="0" t="s">
-        <v>192</v>
+        <v>191</v>
       </c>
       <c r="I68" s="0" t="s">
         <v>18</v>
@@ -3030,28 +3165,28 @@
     </row>
     <row r="69" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A69" s="0" t="s">
+        <v>224</v>
+      </c>
+      <c r="B69" s="0" t="s">
+        <v>11</v>
+      </c>
+      <c r="C69" s="0" t="s">
+        <v>191</v>
+      </c>
+      <c r="D69" s="0" t="s">
+        <v>13</v>
+      </c>
+      <c r="E69" s="0" t="s">
         <v>225</v>
       </c>
-      <c r="B69" s="0" t="s">
-        <v>11</v>
-      </c>
-      <c r="C69" s="0" t="s">
-        <v>192</v>
-      </c>
-      <c r="D69" s="0" t="s">
-        <v>13</v>
-      </c>
-      <c r="E69" s="0" t="s">
+      <c r="F69" s="0" t="s">
         <v>226</v>
       </c>
-      <c r="F69" s="0" t="s">
-        <v>227</v>
-      </c>
       <c r="G69" s="0" t="s">
         <v>16</v>
       </c>
       <c r="H69" s="0" t="s">
-        <v>192</v>
+        <v>191</v>
       </c>
       <c r="I69" s="0" t="s">
         <v>18</v>
@@ -3062,28 +3197,28 @@
     </row>
     <row r="70" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A70" s="0" t="s">
+        <v>227</v>
+      </c>
+      <c r="B70" s="0" t="s">
+        <v>11</v>
+      </c>
+      <c r="C70" s="0" t="s">
+        <v>191</v>
+      </c>
+      <c r="D70" s="0" t="s">
+        <v>13</v>
+      </c>
+      <c r="E70" s="0" t="s">
         <v>228</v>
       </c>
-      <c r="B70" s="0" t="s">
-        <v>11</v>
-      </c>
-      <c r="C70" s="0" t="s">
-        <v>192</v>
-      </c>
-      <c r="D70" s="0" t="s">
-        <v>13</v>
-      </c>
-      <c r="E70" s="0" t="s">
+      <c r="F70" s="0" t="s">
         <v>229</v>
       </c>
-      <c r="F70" s="0" t="s">
-        <v>230</v>
-      </c>
       <c r="G70" s="0" t="s">
         <v>16</v>
       </c>
       <c r="H70" s="0" t="s">
-        <v>192</v>
+        <v>191</v>
       </c>
       <c r="I70" s="0" t="s">
         <v>18</v>
@@ -3094,36 +3229,494 @@
     </row>
     <row r="71" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A71" s="0" t="s">
-        <v>231</v>
+        <v>230</v>
       </c>
       <c r="B71" s="0" t="s">
         <v>11</v>
       </c>
       <c r="C71" s="0" t="s">
-        <v>192</v>
+        <v>191</v>
       </c>
       <c r="D71" s="0" t="s">
         <v>36</v>
       </c>
       <c r="E71" s="0" t="s">
+        <v>231</v>
+      </c>
+      <c r="F71" s="0" t="s">
         <v>232</v>
       </c>
-      <c r="F71" s="0" t="s">
+      <c r="G71" s="0" t="s">
+        <v>16</v>
+      </c>
+      <c r="H71" s="0" t="s">
+        <v>191</v>
+      </c>
+      <c r="I71" s="0" t="s">
+        <v>18</v>
+      </c>
+      <c r="J71" s="0" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="72" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A72" s="0" t="s">
         <v>233</v>
       </c>
-      <c r="G71" s="0" t="s">
-        <v>16</v>
-      </c>
-      <c r="H71" s="0" t="s">
-        <v>192</v>
-      </c>
-      <c r="I71" s="0" t="s">
-        <v>18</v>
-      </c>
-      <c r="J71" s="0" t="s">
-        <v>19</v>
-      </c>
-    </row>
+      <c r="B72" s="0" t="s">
+        <v>11</v>
+      </c>
+      <c r="C72" s="0" t="s">
+        <v>234</v>
+      </c>
+      <c r="D72" s="0" t="s">
+        <v>13</v>
+      </c>
+      <c r="E72" s="0" t="s">
+        <v>235</v>
+      </c>
+      <c r="F72" s="0" t="s">
+        <v>236</v>
+      </c>
+      <c r="G72" s="0" t="s">
+        <v>16</v>
+      </c>
+      <c r="H72" s="0" t="s">
+        <v>237</v>
+      </c>
+      <c r="I72" s="0" t="s">
+        <v>18</v>
+      </c>
+      <c r="J72" s="0" t="s">
+        <v>238</v>
+      </c>
+    </row>
+    <row r="73" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A73" s="0" t="s">
+        <v>239</v>
+      </c>
+      <c r="B73" s="0" t="s">
+        <v>11</v>
+      </c>
+      <c r="C73" s="0" t="s">
+        <v>234</v>
+      </c>
+      <c r="D73" s="0" t="s">
+        <v>13</v>
+      </c>
+      <c r="E73" s="0" t="s">
+        <v>240</v>
+      </c>
+      <c r="F73" s="0" t="s">
+        <v>241</v>
+      </c>
+      <c r="G73" s="0" t="s">
+        <v>16</v>
+      </c>
+      <c r="H73" s="0" t="s">
+        <v>237</v>
+      </c>
+      <c r="I73" s="0" t="s">
+        <v>18</v>
+      </c>
+      <c r="J73" s="0" t="s">
+        <v>238</v>
+      </c>
+    </row>
+    <row r="74" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A74" s="0" t="s">
+        <v>242</v>
+      </c>
+      <c r="B74" s="0" t="s">
+        <v>11</v>
+      </c>
+      <c r="C74" s="0" t="s">
+        <v>234</v>
+      </c>
+      <c r="D74" s="0" t="s">
+        <v>13</v>
+      </c>
+      <c r="E74" s="0" t="s">
+        <v>243</v>
+      </c>
+      <c r="F74" s="0" t="s">
+        <v>244</v>
+      </c>
+      <c r="G74" s="0" t="s">
+        <v>16</v>
+      </c>
+      <c r="H74" s="0" t="s">
+        <v>237</v>
+      </c>
+      <c r="I74" s="0" t="s">
+        <v>18</v>
+      </c>
+      <c r="J74" s="0" t="s">
+        <v>238</v>
+      </c>
+    </row>
+    <row r="75" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A75" s="0" t="s">
+        <v>245</v>
+      </c>
+      <c r="B75" s="0" t="s">
+        <v>11</v>
+      </c>
+      <c r="C75" s="0" t="s">
+        <v>234</v>
+      </c>
+      <c r="D75" s="0" t="s">
+        <v>13</v>
+      </c>
+      <c r="E75" s="0" t="s">
+        <v>246</v>
+      </c>
+      <c r="F75" s="0" t="s">
+        <v>247</v>
+      </c>
+      <c r="G75" s="0" t="s">
+        <v>16</v>
+      </c>
+      <c r="H75" s="0" t="s">
+        <v>237</v>
+      </c>
+      <c r="I75" s="0" t="s">
+        <v>18</v>
+      </c>
+      <c r="J75" s="0" t="s">
+        <v>238</v>
+      </c>
+    </row>
+    <row r="76" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A76" s="0" t="s">
+        <v>248</v>
+      </c>
+      <c r="B76" s="0" t="s">
+        <v>11</v>
+      </c>
+      <c r="C76" s="0" t="s">
+        <v>234</v>
+      </c>
+      <c r="D76" s="0" t="s">
+        <v>13</v>
+      </c>
+      <c r="E76" s="0" t="s">
+        <v>249</v>
+      </c>
+      <c r="F76" s="0" t="s">
+        <v>250</v>
+      </c>
+      <c r="G76" s="0" t="s">
+        <v>16</v>
+      </c>
+      <c r="H76" s="0" t="s">
+        <v>237</v>
+      </c>
+      <c r="I76" s="0" t="s">
+        <v>18</v>
+      </c>
+      <c r="J76" s="0" t="s">
+        <v>238</v>
+      </c>
+    </row>
+    <row r="77" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A77" s="0" t="s">
+        <v>251</v>
+      </c>
+      <c r="B77" s="0" t="s">
+        <v>11</v>
+      </c>
+      <c r="C77" s="0" t="s">
+        <v>234</v>
+      </c>
+      <c r="D77" s="0" t="s">
+        <v>13</v>
+      </c>
+      <c r="E77" s="0" t="s">
+        <v>252</v>
+      </c>
+      <c r="F77" s="0" t="s">
+        <v>253</v>
+      </c>
+      <c r="G77" s="0" t="s">
+        <v>16</v>
+      </c>
+      <c r="H77" s="0" t="s">
+        <v>237</v>
+      </c>
+      <c r="I77" s="0" t="s">
+        <v>18</v>
+      </c>
+      <c r="J77" s="0" t="s">
+        <v>238</v>
+      </c>
+    </row>
+    <row r="78" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A78" s="0" t="s">
+        <v>254</v>
+      </c>
+      <c r="B78" s="0" t="s">
+        <v>11</v>
+      </c>
+      <c r="C78" s="0" t="s">
+        <v>234</v>
+      </c>
+      <c r="D78" s="0" t="s">
+        <v>36</v>
+      </c>
+      <c r="E78" s="0" t="s">
+        <v>255</v>
+      </c>
+      <c r="F78" s="0" t="s">
+        <v>256</v>
+      </c>
+      <c r="G78" s="0" t="s">
+        <v>16</v>
+      </c>
+      <c r="H78" s="0" t="s">
+        <v>237</v>
+      </c>
+      <c r="I78" s="0" t="s">
+        <v>18</v>
+      </c>
+      <c r="J78" s="0" t="s">
+        <v>238</v>
+      </c>
+    </row>
+    <row r="79" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A79" s="0" t="s">
+        <v>257</v>
+      </c>
+      <c r="B79" s="0" t="s">
+        <v>11</v>
+      </c>
+      <c r="C79" s="0" t="s">
+        <v>234</v>
+      </c>
+      <c r="D79" s="0" t="s">
+        <v>13</v>
+      </c>
+      <c r="E79" s="0" t="s">
+        <v>258</v>
+      </c>
+      <c r="F79" s="0" t="s">
+        <v>259</v>
+      </c>
+      <c r="G79" s="0" t="s">
+        <v>16</v>
+      </c>
+      <c r="H79" s="0" t="s">
+        <v>260</v>
+      </c>
+      <c r="I79" s="0" t="s">
+        <v>18</v>
+      </c>
+      <c r="J79" s="0" t="s">
+        <v>238</v>
+      </c>
+    </row>
+    <row r="80" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A80" s="0" t="s">
+        <v>261</v>
+      </c>
+      <c r="B80" s="0" t="s">
+        <v>11</v>
+      </c>
+      <c r="C80" s="0" t="s">
+        <v>234</v>
+      </c>
+      <c r="D80" s="0" t="s">
+        <v>13</v>
+      </c>
+      <c r="E80" s="0" t="s">
+        <v>262</v>
+      </c>
+      <c r="F80" s="0" t="s">
+        <v>263</v>
+      </c>
+      <c r="G80" s="0" t="s">
+        <v>16</v>
+      </c>
+      <c r="H80" s="0" t="s">
+        <v>260</v>
+      </c>
+      <c r="I80" s="0" t="s">
+        <v>18</v>
+      </c>
+      <c r="J80" s="0" t="s">
+        <v>238</v>
+      </c>
+    </row>
+    <row r="81" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A81" s="0" t="s">
+        <v>264</v>
+      </c>
+      <c r="B81" s="0" t="s">
+        <v>11</v>
+      </c>
+      <c r="C81" s="0" t="s">
+        <v>234</v>
+      </c>
+      <c r="D81" s="0" t="s">
+        <v>13</v>
+      </c>
+      <c r="E81" s="0" t="s">
+        <v>265</v>
+      </c>
+      <c r="F81" s="0" t="s">
+        <v>266</v>
+      </c>
+      <c r="G81" s="0" t="s">
+        <v>16</v>
+      </c>
+      <c r="H81" s="0" t="s">
+        <v>260</v>
+      </c>
+      <c r="I81" s="0" t="s">
+        <v>18</v>
+      </c>
+      <c r="J81" s="0" t="s">
+        <v>238</v>
+      </c>
+    </row>
+    <row r="82" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A82" s="0" t="s">
+        <v>267</v>
+      </c>
+      <c r="B82" s="0" t="s">
+        <v>11</v>
+      </c>
+      <c r="C82" s="0" t="s">
+        <v>234</v>
+      </c>
+      <c r="D82" s="0" t="s">
+        <v>13</v>
+      </c>
+      <c r="E82" s="0" t="s">
+        <v>268</v>
+      </c>
+      <c r="F82" s="0" t="s">
+        <v>269</v>
+      </c>
+      <c r="G82" s="0" t="s">
+        <v>16</v>
+      </c>
+      <c r="H82" s="0" t="s">
+        <v>260</v>
+      </c>
+      <c r="I82" s="0" t="s">
+        <v>18</v>
+      </c>
+      <c r="J82" s="0" t="s">
+        <v>238</v>
+      </c>
+    </row>
+    <row r="83" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A83" s="0" t="s">
+        <v>270</v>
+      </c>
+      <c r="B83" s="0" t="s">
+        <v>11</v>
+      </c>
+      <c r="C83" s="0" t="s">
+        <v>234</v>
+      </c>
+      <c r="D83" s="0" t="s">
+        <v>13</v>
+      </c>
+      <c r="E83" s="0" t="s">
+        <v>271</v>
+      </c>
+      <c r="F83" s="0" t="s">
+        <v>272</v>
+      </c>
+      <c r="G83" s="0" t="s">
+        <v>16</v>
+      </c>
+      <c r="H83" s="0" t="s">
+        <v>260</v>
+      </c>
+      <c r="I83" s="0" t="s">
+        <v>18</v>
+      </c>
+      <c r="J83" s="0" t="s">
+        <v>238</v>
+      </c>
+    </row>
+    <row r="84" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A84" s="0" t="s">
+        <v>273</v>
+      </c>
+      <c r="B84" s="0" t="s">
+        <v>11</v>
+      </c>
+      <c r="C84" s="0" t="s">
+        <v>234</v>
+      </c>
+      <c r="D84" s="0" t="s">
+        <v>13</v>
+      </c>
+      <c r="E84" s="0" t="s">
+        <v>274</v>
+      </c>
+      <c r="F84" s="0" t="s">
+        <v>275</v>
+      </c>
+      <c r="G84" s="0" t="s">
+        <v>16</v>
+      </c>
+      <c r="H84" s="0" t="s">
+        <v>260</v>
+      </c>
+      <c r="I84" s="0" t="s">
+        <v>18</v>
+      </c>
+      <c r="J84" s="0" t="s">
+        <v>238</v>
+      </c>
+    </row>
+    <row r="85" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A85" s="0" t="s">
+        <v>276</v>
+      </c>
+      <c r="B85" s="0" t="s">
+        <v>11</v>
+      </c>
+      <c r="C85" s="0" t="s">
+        <v>234</v>
+      </c>
+      <c r="D85" s="0" t="s">
+        <v>36</v>
+      </c>
+      <c r="E85" s="0" t="s">
+        <v>277</v>
+      </c>
+      <c r="F85" s="0" t="s">
+        <v>278</v>
+      </c>
+      <c r="G85" s="0" t="s">
+        <v>16</v>
+      </c>
+      <c r="H85" s="0" t="s">
+        <v>260</v>
+      </c>
+      <c r="I85" s="0" t="s">
+        <v>18</v>
+      </c>
+      <c r="J85" s="0" t="s">
+        <v>238</v>
+      </c>
+    </row>
+    <row r="86" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="87" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="88" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="89" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
+    <row r="94" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="F94" s="0" t="s">
+        <v>238</v>
+      </c>
+    </row>
+    <row r="1048576" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false"/>
   </sheetData>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.7875" right="0.7875" top="1.05277777777778" bottom="1.05277777777778" header="0.7875" footer="0.7875"/>

</xml_diff>